<commit_message>
j'ai corrigé un bug
</commit_message>
<xml_diff>
--- a/planning/static/excel/planning.xlsx
+++ b/planning/static/excel/planning.xlsx
@@ -47,8 +47,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
     <fill>
@@ -59,14 +65,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor rgb="FF99FF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -105,11 +105,11 @@
   <cellXfs count="9">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -488,24 +488,24 @@
     <col customWidth="1" max="1" min="1" width="14.4"/>
     <col customWidth="1" max="2" min="2" width="25.2"/>
     <col customWidth="1" max="3" min="3" width="27.6"/>
-    <col customWidth="1" max="4" min="4" width="28.8"/>
+    <col customWidth="1" max="4" min="4" width="22.8"/>
     <col customWidth="1" max="5" min="5" width="28.8"/>
     <col customWidth="1" max="6" min="6" width="7.199999999999999"/>
-    <col customWidth="1" max="7" min="7" width="27.6"/>
+    <col customWidth="1" max="7" min="7" width="28.8"/>
     <col customWidth="1" max="8" min="8" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Semaine 36</t>
+          <t>Semaine 33</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>JEUDI</t>
+          <t>LUNDI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -541,9 +541,9 @@
           <t>B 1604</t>
         </is>
       </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>HELFTER Franck</t>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
       <c r="E4" s="3" t="inlineStr">
@@ -551,21 +551,21 @@
           <t>BROGLIE Julien</t>
         </is>
       </c>
-      <c r="G4" s="3" t="inlineStr">
-        <is>
-          <t>MULLER Gilbert</t>
+      <c r="G4" s="4" t="inlineStr">
+        <is>
+          <t>DA SILVA David</t>
         </is>
       </c>
       <c r="H4" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>SCHILLINGER  Jérémy</t>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>HORACEK Julien</t>
         </is>
       </c>
       <c r="E5" s="3" t="inlineStr">
@@ -575,19 +575,19 @@
       </c>
     </row>
     <row r="6">
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>CAMARASA Sébastien</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>SIMON Gael</t>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>HUEBER Olivier</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>WITZ Alain</t>
         </is>
       </c>
       <c r="G6" s="3" t="inlineStr">
         <is>
-          <t>SCHAAL Eric</t>
+          <t>FRICKERT Rémy</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -603,43 +603,33 @@
           <t>B 2100</t>
         </is>
       </c>
-      <c r="C8" s="4" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
         <is>
           <t>LUDAESCHER Olivier</t>
         </is>
       </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>DUCROT Déborah</t>
-        </is>
-      </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
           <t>MORENO José</t>
         </is>
       </c>
-      <c r="G8" s="5" t="inlineStr">
-        <is>
-          <t>DA SILVA David</t>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>ACKERMANN Rémy</t>
         </is>
       </c>
       <c r="H8" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>F</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="4" t="inlineStr">
+      <c r="C9" s="2" t="inlineStr">
         <is>
           <t>HAAG Patrick</t>
         </is>
       </c>
-      <c r="D9" s="2" t="inlineStr">
-        <is>
-          <t>ROUSSIN Frédéric</t>
-        </is>
-      </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
           <t>ABELLAN GRINAN Laurent</t>
@@ -647,24 +637,19 @@
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="4" t="inlineStr">
-        <is>
-          <t>HORACEK Julien</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>BLATZ Jean-Marie</t>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>SIMON Gael</t>
         </is>
       </c>
       <c r="E10" s="3" t="inlineStr">
         <is>
-          <t>DA COSTA Nelson</t>
-        </is>
-      </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>FRICKERT Rémy</t>
+          <t>SCHAAL Eric</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>CAMACHO Michel</t>
         </is>
       </c>
       <c r="H10" s="1" t="inlineStr">
@@ -680,43 +665,33 @@
           <t>B2000</t>
         </is>
       </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
         <is>
           <t>SIGWALT Thierry</t>
         </is>
       </c>
-      <c r="E12" s="3" t="inlineStr">
-        <is>
-          <t>RUBIO Alexandre</t>
-        </is>
-      </c>
-      <c r="G12" s="3" t="inlineStr">
-        <is>
-          <t>GAVROY Gilles</t>
+      <c r="G12" s="2" t="inlineStr">
+        <is>
+          <t>ROGLER Richard</t>
         </is>
       </c>
       <c r="H12" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="E13" s="3" t="inlineStr">
-        <is>
-          <t>WITZ Alain</t>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOIREAU Stéphane </t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="G14" s="3" t="inlineStr">
-        <is>
-          <t>KIEFFER Victor</t>
+      <c r="G14" s="6" t="inlineStr">
+        <is>
+          <t>CAMARASA Sébastien</t>
         </is>
       </c>
       <c r="H14" s="1" t="inlineStr">
@@ -732,24 +707,19 @@
           <t>G 1628</t>
         </is>
       </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
         <is>
           <t>BUCHER Cyril</t>
         </is>
       </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>NESZCZADYN Franck</t>
-        </is>
-      </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
           <t>FOECHTERLE Jean</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr">
-        <is>
-          <t>RIGOT Sébastien</t>
+      <c r="G16" s="6" t="inlineStr">
+        <is>
+          <t>PASQUIER Alexandre</t>
         </is>
       </c>
       <c r="H16" s="1" t="inlineStr">
@@ -759,16 +729,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="4" t="inlineStr">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>GEIGER Frédéric</t>
         </is>
       </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Pascal</t>
-        </is>
-      </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
           <t>FULLERINGER Gaétan</t>
@@ -776,24 +741,19 @@
       </c>
     </row>
     <row r="18">
-      <c r="C18" s="4" t="inlineStr">
-        <is>
-          <t>VINGATARAMIN Pierre</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>LICHTLE Jean-Sébastien</t>
-        </is>
-      </c>
-      <c r="E18" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>SAHLI Halim</t>
+        </is>
+      </c>
+      <c r="E18" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
         </is>
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>WOELFFLIN Gregory</t>
+          <t xml:space="preserve">KOESSEL Marc </t>
         </is>
       </c>
       <c r="H18" s="1" t="inlineStr">
@@ -809,45 +769,29 @@
           <t>DOMINO</t>
         </is>
       </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>BAUMANN Dylan</t>
         </is>
       </c>
-      <c r="D20" s="2" t="inlineStr">
-        <is>
-          <t>BERGER Virgil</t>
-        </is>
-      </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
           <t>SPIELMANN Patrice</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr">
-        <is>
-          <t>CAMACHO Michel</t>
+      <c r="G20" s="6" t="inlineStr">
+        <is>
+          <t>LUDAESCHER Pascal</t>
         </is>
       </c>
       <c r="H20" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
     <row r="21"/>
-    <row r="22">
-      <c r="G22" s="4" t="inlineStr">
-        <is>
-          <t>FRILLOT Jacky</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-    </row>
+    <row r="22"/>
     <row r="23"/>
     <row r="24">
       <c r="B24" s="1" t="inlineStr">
@@ -855,42 +799,27 @@
           <t>PRESSE À BALLE</t>
         </is>
       </c>
-      <c r="C24" s="4" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
         <is>
           <t>SCHREIBER Bertrand</t>
         </is>
       </c>
-      <c r="D24" s="2" t="inlineStr">
+      <c r="D24" s="6" t="inlineStr">
         <is>
           <t>CORSET Christo</t>
         </is>
       </c>
       <c r="E24" s="3" t="inlineStr">
         <is>
-          <t>SCHENCK Emmanuel</t>
-        </is>
-      </c>
-      <c r="G24" s="4" t="inlineStr">
-        <is>
-          <t>FUCHS Eric</t>
-        </is>
-      </c>
-      <c r="H24" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+          <t>MULLER Gilbert</t>
         </is>
       </c>
     </row>
     <row r="25"/>
     <row r="26">
-      <c r="G26" s="4" t="inlineStr">
-        <is>
-          <t>HAIL Fehrat</t>
-        </is>
-      </c>
-      <c r="H26" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Personnel non affecté</t>
         </is>
       </c>
     </row>
@@ -901,27 +830,17 @@
           <t>PLATEAUX</t>
         </is>
       </c>
-      <c r="G28" s="4" t="inlineStr">
-        <is>
-          <t>ROSSE Madeline</t>
-        </is>
-      </c>
-      <c r="H28" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G28" s="2" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
         </is>
       </c>
     </row>
     <row r="29"/>
     <row r="30">
-      <c r="G30" s="4" t="inlineStr">
-        <is>
-          <t>SAHLI Halim</t>
-        </is>
-      </c>
-      <c r="H30" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G30" s="6" t="inlineStr">
+        <is>
+          <t>BERGER Virgil</t>
         </is>
       </c>
     </row>
@@ -932,42 +851,27 @@
           <t>EMBALLAGE</t>
         </is>
       </c>
-      <c r="C32" s="4" t="inlineStr">
+      <c r="C32" s="2" t="inlineStr">
         <is>
           <t>SUTTER Thierry</t>
         </is>
       </c>
-      <c r="D32" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ROTH Mathieu </t>
-        </is>
-      </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
           <t>GANTNER Stéphane</t>
         </is>
       </c>
-      <c r="G32" s="2" t="inlineStr">
-        <is>
-          <t>LEROY Nicolas</t>
-        </is>
-      </c>
-      <c r="H32" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G32" s="6" t="inlineStr">
+        <is>
+          <t>BIELLMANN Cindy</t>
         </is>
       </c>
     </row>
     <row r="33"/>
     <row r="34">
-      <c r="G34" s="2" t="inlineStr">
-        <is>
-          <t>SCANDELLA Christophe</t>
-        </is>
-      </c>
-      <c r="H34" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G34" s="6" t="inlineStr">
+        <is>
+          <t>DA SILVA Axel</t>
         </is>
       </c>
     </row>
@@ -978,14 +882,14 @@
           <t>MANUTENTION LOURD</t>
         </is>
       </c>
-      <c r="C36" s="4" t="inlineStr">
+      <c r="C36" s="2" t="inlineStr">
         <is>
           <t>MOEGLING Vincent</t>
         </is>
       </c>
-      <c r="D36" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BOIREAU Stéphane </t>
+      <c r="D36" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DJEBARA Philippe </t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
@@ -995,17 +899,18 @@
       </c>
       <c r="G36" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
-        </is>
-      </c>
-      <c r="H36" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+          <t>DUCROT Déborah</t>
         </is>
       </c>
     </row>
     <row r="37"/>
-    <row r="38"/>
+    <row r="38">
+      <c r="G38" s="6" t="inlineStr">
+        <is>
+          <t>GRIMONT Olivier</t>
+        </is>
+      </c>
+    </row>
     <row r="39"/>
     <row r="40">
       <c r="B40" s="1" t="inlineStr">
@@ -1015,20 +920,25 @@
       </c>
       <c r="C40" s="7" t="inlineStr">
         <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="D40" s="8" t="inlineStr">
-        <is>
           <t>Vincent WENDLING</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
+        </is>
+      </c>
+      <c r="G40" s="6" t="inlineStr">
+        <is>
+          <t>GUMUS Fatih</t>
         </is>
       </c>
     </row>
     <row r="41"/>
     <row r="42">
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>Personnel non affecté</t>
+      <c r="G42" s="6" t="inlineStr">
+        <is>
+          <t>HELFTER Franck</t>
         </is>
       </c>
     </row>
@@ -1039,48 +949,33 @@
           <t>M 1848/1</t>
         </is>
       </c>
-      <c r="C44" s="4" t="inlineStr">
+      <c r="C44" s="2" t="inlineStr">
         <is>
           <t>NETALA Frédéric</t>
         </is>
       </c>
-      <c r="E44" s="3" t="inlineStr">
-        <is>
-          <t>FRICKERT Florian</t>
-        </is>
-      </c>
       <c r="G44" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">DJEBARA Philippe </t>
+          <t>LICHTLE Jean-Sébastien</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="4" t="inlineStr">
-        <is>
-          <t>LEDER Frédéric</t>
-        </is>
-      </c>
-      <c r="E45" s="3" t="inlineStr">
-        <is>
-          <t>SPITZ Eric</t>
+      <c r="C45" s="2" t="inlineStr">
+        <is>
+          <t>FRILLOT Jacky</t>
         </is>
       </c>
     </row>
     <row r="46">
-      <c r="C46" s="4" t="inlineStr">
+      <c r="C46" s="2" t="inlineStr">
         <is>
           <t>HUGG Christian</t>
         </is>
       </c>
-      <c r="E46" s="3" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
-        </is>
-      </c>
       <c r="G46" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">PINTO José </t>
+          <t>ROUSSIN Frédéric</t>
         </is>
       </c>
     </row>
@@ -1091,14 +986,9 @@
           <t>M 1848/2</t>
         </is>
       </c>
-      <c r="C48" s="4" t="inlineStr">
-        <is>
-          <t>AUDREN Olivier</t>
-        </is>
-      </c>
-      <c r="D48" s="2" t="inlineStr">
-        <is>
-          <t>GRIMONT Olivier</t>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>FUCHS Eric</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
@@ -1106,16 +996,16 @@
           <t>VILLEMIN Franck</t>
         </is>
       </c>
+      <c r="G48" s="6" t="inlineStr">
+        <is>
+          <t>SCANDELLA Christophe</t>
+        </is>
+      </c>
     </row>
     <row r="49">
-      <c r="C49" s="4" t="inlineStr">
+      <c r="C49" s="2" t="inlineStr">
         <is>
           <t>FONTAINE Fabien</t>
-        </is>
-      </c>
-      <c r="D49" s="2" t="inlineStr">
-        <is>
-          <t>DA SILVA Axel</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
@@ -1127,17 +1017,17 @@
     <row r="50">
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>Intérimaire</t>
-        </is>
-      </c>
-      <c r="D50" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
+          <t>AUDREN Olivier</t>
         </is>
       </c>
       <c r="E50" s="3" t="inlineStr">
         <is>
-          <t>FIGUEIREDO José</t>
+          <t>FRICKERT Florian</t>
+        </is>
+      </c>
+      <c r="G50" s="6" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
         </is>
       </c>
     </row>
@@ -1148,30 +1038,31 @@
           <t>TCY</t>
         </is>
       </c>
-      <c r="C52" s="2" t="inlineStr">
-        <is>
-          <t>SCHWARZ Jean-Philippe</t>
-        </is>
-      </c>
-      <c r="E52" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>KIEFFER Victor</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PINTO José </t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="C53" s="3" t="inlineStr">
+      <c r="E53" s="3" t="inlineStr">
         <is>
           <t>MOZET Gaétan</t>
         </is>
       </c>
-      <c r="E53" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-    </row>
-    <row r="54"/>
+    </row>
+    <row r="54">
+      <c r="G54" s="3" t="inlineStr">
+        <is>
+          <t>DA COSTA Nelson</t>
+        </is>
+      </c>
+    </row>
     <row r="55"/>
     <row r="56">
       <c r="B56" s="1" t="inlineStr">
@@ -1179,14 +1070,20 @@
           <t>SRE</t>
         </is>
       </c>
-      <c r="C56" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="G56" s="3" t="inlineStr">
+        <is>
+          <t>FIGUEIREDO José</t>
         </is>
       </c>
     </row>
     <row r="57"/>
-    <row r="58"/>
+    <row r="58">
+      <c r="G58" s="3" t="inlineStr">
+        <is>
+          <t>GAVROY Gilles</t>
+        </is>
+      </c>
+    </row>
     <row r="59"/>
     <row r="60">
       <c r="B60" s="1" t="inlineStr">
@@ -1194,14 +1091,25 @@
           <t>SMT</t>
         </is>
       </c>
-      <c r="C60" s="4" t="inlineStr">
+      <c r="C60" s="2" t="inlineStr">
         <is>
           <t>BELIANE Karim</t>
         </is>
       </c>
+      <c r="G60" s="3" t="inlineStr">
+        <is>
+          <t>LOUIS Nicolas</t>
+        </is>
+      </c>
     </row>
     <row r="61"/>
-    <row r="62"/>
+    <row r="62">
+      <c r="G62" s="3" t="inlineStr">
+        <is>
+          <t>RENCKER Michel</t>
+        </is>
+      </c>
+    </row>
     <row r="63"/>
     <row r="64">
       <c r="B64" s="1" t="inlineStr">
@@ -1209,14 +1117,25 @@
           <t>LBB1</t>
         </is>
       </c>
-      <c r="C64" s="4" t="inlineStr">
-        <is>
-          <t>BELIANE Karim</t>
+      <c r="C64" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ROTH Mathieu </t>
+        </is>
+      </c>
+      <c r="G64" s="3" t="inlineStr">
+        <is>
+          <t>RUBIO Alexandre</t>
         </is>
       </c>
     </row>
     <row r="65"/>
-    <row r="66"/>
+    <row r="66">
+      <c r="G66" s="3" t="inlineStr">
+        <is>
+          <t>SPITZ Eric</t>
+        </is>
+      </c>
+    </row>
     <row r="67"/>
     <row r="68">
       <c r="B68" s="1" t="inlineStr">
@@ -1244,12 +1163,12 @@
           <t>MANUTENTION INTÉGRÉ</t>
         </is>
       </c>
-      <c r="C76" s="4" t="inlineStr">
+      <c r="C76" s="2" t="inlineStr">
         <is>
           <t>RAMON Dominique</t>
         </is>
       </c>
-      <c r="D76" s="2" t="inlineStr">
+      <c r="D76" s="6" t="inlineStr">
         <is>
           <t>BAUMANN Mike</t>
         </is>
@@ -1269,12 +1188,12 @@
           <t>PRÉPARATEUR</t>
         </is>
       </c>
-      <c r="C80" s="4" t="inlineStr">
+      <c r="C80" s="2" t="inlineStr">
         <is>
           <t>CASPAR Gaël</t>
         </is>
       </c>
-      <c r="D80" s="2" t="inlineStr">
+      <c r="D80" s="6" t="inlineStr">
         <is>
           <t>HERMANN Cédric</t>
         </is>
@@ -1294,26 +1213,16 @@
           <t>M 1228</t>
         </is>
       </c>
-      <c r="C84" s="3" t="inlineStr">
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>HAIL Fehrat</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="C85" s="3" t="inlineStr">
         <is>
           <t>GURLER Onur</t>
-        </is>
-      </c>
-      <c r="D84" s="2" t="inlineStr">
-        <is>
-          <t>GRASSIN Axel</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="C85" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="D85" s="2" t="inlineStr">
-        <is>
-          <t>FRITSCH Julien</t>
         </is>
       </c>
     </row>
@@ -1325,16 +1234,11 @@
           <t>M 924</t>
         </is>
       </c>
-      <c r="C88" s="4" t="inlineStr">
+      <c r="C88" s="2" t="inlineStr">
         <is>
           <t>HIRSINGER Pascal</t>
         </is>
       </c>
-      <c r="D88" s="2" t="inlineStr">
-        <is>
-          <t>ANDRZEJEWSKI Nicolas</t>
-        </is>
-      </c>
       <c r="E88" s="3" t="inlineStr">
         <is>
           <t>RUDLOFF Jérémy</t>
@@ -1342,19 +1246,14 @@
       </c>
     </row>
     <row r="89">
-      <c r="C89" s="4" t="inlineStr">
+      <c r="C89" s="2" t="inlineStr">
         <is>
           <t>HILDWEIN Steve</t>
         </is>
       </c>
-      <c r="D89" s="2" t="inlineStr">
-        <is>
-          <t>BIELLMANN Cindy</t>
-        </is>
-      </c>
-      <c r="E89" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="E89" s="3" t="inlineStr">
+        <is>
+          <t>CORNOT David</t>
         </is>
       </c>
     </row>
@@ -1366,16 +1265,11 @@
           <t>M 718</t>
         </is>
       </c>
-      <c r="C92" s="4" t="inlineStr">
+      <c r="C92" s="2" t="inlineStr">
         <is>
           <t>RAKOTONDRAMANANA Nivo</t>
         </is>
       </c>
-      <c r="D92" s="2" t="inlineStr">
-        <is>
-          <t>MASSINON Frédéric</t>
-        </is>
-      </c>
       <c r="E92" s="3" t="inlineStr">
         <is>
           <t>FERDER Thomas</t>
@@ -1383,14 +1277,9 @@
       </c>
     </row>
     <row r="93">
-      <c r="C93" s="4" t="inlineStr">
-        <is>
-          <t>ACKERMANN Rémy</t>
-        </is>
-      </c>
-      <c r="D93" s="2" t="inlineStr">
-        <is>
-          <t>PASQUIER Alexandre</t>
+      <c r="C93" s="3" t="inlineStr">
+        <is>
+          <t>LIER Romain</t>
         </is>
       </c>
       <c r="E93" s="3" t="inlineStr">
@@ -1407,36 +1296,16 @@
           <t>LMC</t>
         </is>
       </c>
-      <c r="C96" s="4" t="inlineStr">
+      <c r="C96" s="2" t="inlineStr">
         <is>
           <t>EBRAN Vincent</t>
         </is>
       </c>
-      <c r="D96" s="2" t="inlineStr">
-        <is>
-          <t>GIDEMANN Olivier</t>
-        </is>
-      </c>
-      <c r="E96" s="3" t="inlineStr">
-        <is>
-          <t>CORNOT David</t>
-        </is>
-      </c>
     </row>
     <row r="97">
-      <c r="C97" s="3" t="inlineStr">
-        <is>
-          <t>LOUIS Nicolas</t>
-        </is>
-      </c>
-      <c r="D97" s="7" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="E97" s="3" t="inlineStr">
-        <is>
-          <t>LIER Romain</t>
+      <c r="C97" s="2" t="inlineStr">
+        <is>
+          <t>ROSSE Madeline</t>
         </is>
       </c>
     </row>
@@ -1448,12 +1317,12 @@
           <t>CENTRE-POSE</t>
         </is>
       </c>
-      <c r="C100" s="4" t="inlineStr">
-        <is>
-          <t>ROGLER Richard</t>
-        </is>
-      </c>
-      <c r="D100" s="2" t="inlineStr">
+      <c r="C100" s="6" t="inlineStr">
+        <is>
+          <t>GRASSIN Axel</t>
+        </is>
+      </c>
+      <c r="D100" s="6" t="inlineStr">
         <is>
           <t>WEHRLEN Patrice</t>
         </is>
@@ -1475,6 +1344,11 @@
       </c>
       <c r="C104" s="2" t="inlineStr">
         <is>
+          <t>RIGOT Sébastien</t>
+        </is>
+      </c>
+      <c r="D104" s="6" t="inlineStr">
+        <is>
           <t>VIAUD Cyril</t>
         </is>
       </c>
@@ -1488,7 +1362,7 @@
           <t>HST</t>
         </is>
       </c>
-      <c r="C108" s="7" t="inlineStr">
+      <c r="C108" s="8" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>

</xml_diff>

<commit_message>
changement sur le fichier excel
</commit_message>
<xml_diff>
--- a/planning/static/excel/planning.xlsx
+++ b/planning/static/excel/planning.xlsx
@@ -35,8 +35,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6D6D"/>
-        <bgColor rgb="FFFF6D6D"/>
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -53,20 +59,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor rgb="FF99FF99"/>
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6D6D"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
     <fill>
@@ -106,12 +106,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H108"/>
+  <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,26 +486,31 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="14.4"/>
-    <col customWidth="1" max="2" min="2" width="25.2"/>
-    <col customWidth="1" max="3" min="3" width="27.6"/>
-    <col customWidth="1" max="4" min="4" width="22.8"/>
+    <col customWidth="1" max="2" min="2" width="22.8"/>
+    <col customWidth="1" max="3" min="3" width="28.8"/>
+    <col customWidth="1" max="4" min="4" width="25.2"/>
     <col customWidth="1" max="5" min="5" width="28.8"/>
     <col customWidth="1" max="6" min="6" width="7.199999999999999"/>
-    <col customWidth="1" max="7" min="7" width="28.8"/>
-    <col customWidth="1" max="8" min="8" width="9.6"/>
+    <col customWidth="1" max="7" min="7" width="25.2"/>
+    <col customWidth="1" max="8" min="8" width="26.4"/>
+    <col customWidth="1" max="9" min="9" width="27.6"/>
+    <col customWidth="1" max="10" min="10" width="22.8"/>
+    <col customWidth="1" max="11" min="11" width="7.199999999999999"/>
+    <col customWidth="1" max="12" min="12" width="27.6"/>
+    <col customWidth="1" max="13" min="13" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Semaine 33</t>
+          <t>Semaine 19</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LUNDI</t>
+          <t>MERCREDI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -523,12 +528,27 @@
           <t>Nuit</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" s="1" t="inlineStr">
+        <is>
+          <t>Matin</t>
+        </is>
+      </c>
+      <c r="I2" s="1" t="inlineStr">
+        <is>
+          <t>Après-midi</t>
+        </is>
+      </c>
+      <c r="J2" s="1" t="inlineStr">
+        <is>
+          <t>Nuit</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
         <is>
           <t>Nom</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Raison</t>
         </is>
@@ -543,20 +563,40 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
+          <t>HELFTER Franck</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
           <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
-      <c r="E4" s="3" t="inlineStr">
+      <c r="E4" s="4" t="inlineStr">
         <is>
           <t>BROGLIE Julien</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr">
-        <is>
-          <t>DA SILVA David</t>
-        </is>
-      </c>
-      <c r="H4" s="1" t="inlineStr">
+      <c r="G4" s="1" t="inlineStr">
+        <is>
+          <t>SMT</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ROTH Mathieu </t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DJEBARA Philippe </t>
+        </is>
+      </c>
+      <c r="L4" s="4" t="inlineStr">
+        <is>
+          <t>DA COSTA Nelson</t>
+        </is>
+      </c>
+      <c r="M4" s="1" t="inlineStr">
         <is>
           <t>M</t>
         </is>
@@ -565,32 +605,42 @@
     <row r="5">
       <c r="C5" s="2" t="inlineStr">
         <is>
+          <t>SCHILLINGER  Jérémy</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
           <t>HORACEK Julien</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>YEGEN Zulkifar</t>
+      <c r="E5" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="2" t="inlineStr">
         <is>
+          <t>CAMARASA Sébastien</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
           <t>HUEBER Olivier</t>
         </is>
       </c>
-      <c r="E6" s="3" t="inlineStr">
-        <is>
-          <t>WITZ Alain</t>
-        </is>
-      </c>
-      <c r="G6" s="3" t="inlineStr">
-        <is>
-          <t>FRICKERT Rémy</t>
-        </is>
-      </c>
-      <c r="H6" s="1" t="inlineStr">
+      <c r="E6" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="inlineStr">
+        <is>
+          <t>FULLERINGER Gaétan</t>
+        </is>
+      </c>
+      <c r="M6" s="1" t="inlineStr">
         <is>
           <t>C</t>
         </is>
@@ -605,32 +655,47 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
+          <t>DUCROT Déborah</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
           <t>LUDAESCHER Olivier</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="4" t="inlineStr">
         <is>
           <t>MORENO José</t>
         </is>
       </c>
-      <c r="G8" s="2" t="inlineStr">
-        <is>
-          <t>ACKERMANN Rémy</t>
-        </is>
-      </c>
-      <c r="H8" s="1" t="inlineStr">
-        <is>
-          <t>F</t>
+      <c r="G8" s="1" t="inlineStr">
+        <is>
+          <t>LBB1</t>
+        </is>
+      </c>
+      <c r="L8" s="4" t="inlineStr">
+        <is>
+          <t>LOUIS Nicolas</t>
+        </is>
+      </c>
+      <c r="M8" s="1" t="inlineStr">
+        <is>
+          <t>rcn</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="C9" s="2" t="inlineStr">
         <is>
+          <t>ROUSSIN Frédéric</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
           <t>HAAG Patrick</t>
         </is>
       </c>
-      <c r="E9" s="3" t="inlineStr">
+      <c r="E9" s="4" t="inlineStr">
         <is>
           <t>ABELLAN GRINAN Laurent</t>
         </is>
@@ -639,22 +704,27 @@
     <row r="10">
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>SIMON Gael</t>
-        </is>
-      </c>
-      <c r="E10" s="3" t="inlineStr">
+          <t>LICHTLE Jean-Sébastien</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
         <is>
           <t>SCHAAL Eric</t>
         </is>
       </c>
-      <c r="G10" s="2" t="inlineStr">
-        <is>
-          <t>CAMACHO Michel</t>
-        </is>
-      </c>
-      <c r="H10" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="L10" s="4" t="inlineStr">
+        <is>
+          <t>MOSCOPOULOS Sébastien</t>
+        </is>
+      </c>
+      <c r="M10" s="1" t="inlineStr">
+        <is>
+          <t>rcn</t>
         </is>
       </c>
     </row>
@@ -665,38 +735,48 @@
           <t>B2000</t>
         </is>
       </c>
-      <c r="C12" s="2" t="inlineStr">
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>SIGWALT Thierry</t>
         </is>
       </c>
-      <c r="G12" s="2" t="inlineStr">
-        <is>
-          <t>ROGLER Richard</t>
-        </is>
-      </c>
-      <c r="H12" s="1" t="inlineStr">
-        <is>
-          <t>D</t>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>MITRAILLEUSE</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PINTO José </t>
+        </is>
+      </c>
+      <c r="L12" s="4" t="inlineStr">
+        <is>
+          <t>SPIELMANN Patrice</t>
+        </is>
+      </c>
+      <c r="M12" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BOIREAU Stéphane </t>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>NESZCZADYN Franck</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="G14" s="6" t="inlineStr">
-        <is>
-          <t>CAMARASA Sébastien</t>
-        </is>
-      </c>
-      <c r="H14" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="L14" s="4" t="inlineStr">
+        <is>
+          <t>TRAPANESE Antoine</t>
+        </is>
+      </c>
+      <c r="M14" s="1" t="inlineStr">
+        <is>
+          <t>rcn</t>
         </is>
       </c>
     </row>
@@ -707,58 +787,63 @@
           <t>G 1628</t>
         </is>
       </c>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>BUCHER Cyril</t>
-        </is>
-      </c>
-      <c r="E16" s="3" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
         <is>
           <t>FOECHTERLE Jean</t>
         </is>
       </c>
-      <c r="G16" s="6" t="inlineStr">
-        <is>
-          <t>PASQUIER Alexandre</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>MITR. BIMAC</t>
+        </is>
+      </c>
+      <c r="L16" s="4" t="inlineStr">
+        <is>
+          <t>WITZ Alain</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="C17" s="2" t="inlineStr">
+      <c r="D17" s="3" t="inlineStr">
         <is>
           <t>GEIGER Frédéric</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr">
-        <is>
-          <t>FULLERINGER Gaétan</t>
+      <c r="E17" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>SAHLI Halim</t>
-        </is>
-      </c>
-      <c r="E18" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="G18" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
-        </is>
-      </c>
-      <c r="H18" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="E18" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L18" s="4" t="inlineStr">
+        <is>
+          <t>YEGEN Zulkifar</t>
+        </is>
+      </c>
+      <c r="M18" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -771,27 +856,63 @@
       </c>
       <c r="C20" s="2" t="inlineStr">
         <is>
+          <t>BERGER Virgil</t>
+        </is>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
           <t>BAUMANN Dylan</t>
         </is>
       </c>
-      <c r="E20" s="3" t="inlineStr">
-        <is>
-          <t>SPIELMANN Patrice</t>
-        </is>
-      </c>
-      <c r="G20" s="6" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Pascal</t>
-        </is>
-      </c>
-      <c r="H20" s="1" t="inlineStr">
-        <is>
-          <t>D</t>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KOESSEL Marc </t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>MANUTENTION INTÉGRÉ</t>
+        </is>
+      </c>
+      <c r="H20" s="2" t="inlineStr">
+        <is>
+          <t>BAUMANN Mike</t>
+        </is>
+      </c>
+      <c r="I20" s="3" t="inlineStr">
+        <is>
+          <t>RAMON Dominique</t>
+        </is>
+      </c>
+      <c r="J20" s="4" t="inlineStr">
+        <is>
+          <t>HOFFERT Patrick</t>
+        </is>
+      </c>
+      <c r="L20" s="7" t="inlineStr">
+        <is>
+          <t>DA SILVA David</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="21"/>
-    <row r="22"/>
+    <row r="22">
+      <c r="L22" s="4" t="inlineStr">
+        <is>
+          <t>FERDER Thomas</t>
+        </is>
+      </c>
+      <c r="M22" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
     <row r="23"/>
     <row r="24">
       <c r="B24" s="1" t="inlineStr">
@@ -799,27 +920,62 @@
           <t>PRESSE À BALLE</t>
         </is>
       </c>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>SCHREIBER Bertrand</t>
+      <c r="C24" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="D24" s="6" t="inlineStr">
         <is>
-          <t>CORSET Christo</t>
-        </is>
-      </c>
-      <c r="E24" s="3" t="inlineStr">
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
         <is>
           <t>MULLER Gilbert</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>PRÉPARATEUR</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>HERMANN Cédric</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>CASPAR Gaël</t>
+        </is>
+      </c>
+      <c r="J24" s="4" t="inlineStr">
+        <is>
+          <t>RITT Jean Jacques</t>
+        </is>
+      </c>
+      <c r="L24" s="7" t="inlineStr">
+        <is>
+          <t>GURLER ONUR</t>
+        </is>
+      </c>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="25"/>
     <row r="26">
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Personnel non affecté</t>
+      <c r="L26" s="4" t="inlineStr">
+        <is>
+          <t>LIER Romain</t>
+        </is>
+      </c>
+      <c r="M26" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
@@ -830,17 +986,53 @@
           <t>PLATEAUX</t>
         </is>
       </c>
-      <c r="G28" s="2" t="inlineStr">
-        <is>
-          <t>LEDER Frédéric</t>
-        </is>
-      </c>
-    </row>
-    <row r="29"/>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>M 1228</t>
+        </is>
+      </c>
+      <c r="H28" s="2" t="inlineStr">
+        <is>
+          <t>GRASSIN Axel</t>
+        </is>
+      </c>
+      <c r="J28" s="4" t="inlineStr">
+        <is>
+          <t>FRICKERT Rémy</t>
+        </is>
+      </c>
+      <c r="L28" s="4" t="inlineStr">
+        <is>
+          <t>VILLEMIN Franck</t>
+        </is>
+      </c>
+      <c r="M28" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="J29" s="4" t="inlineStr">
+        <is>
+          <t>GURLER Onur</t>
+        </is>
+      </c>
+    </row>
     <row r="30">
-      <c r="G30" s="6" t="inlineStr">
-        <is>
-          <t>BERGER Virgil</t>
+      <c r="L30" s="3" t="inlineStr">
+        <is>
+          <t>BUCHER Cyril</t>
+        </is>
+      </c>
+      <c r="M30" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -853,25 +1045,76 @@
       </c>
       <c r="C32" s="2" t="inlineStr">
         <is>
+          <t>LEROY Nicolas</t>
+        </is>
+      </c>
+      <c r="D32" s="3" t="inlineStr">
+        <is>
           <t>SUTTER Thierry</t>
         </is>
       </c>
-      <c r="E32" s="3" t="inlineStr">
+      <c r="E32" s="4" t="inlineStr">
         <is>
           <t>GANTNER Stéphane</t>
         </is>
       </c>
-      <c r="G32" s="6" t="inlineStr">
-        <is>
-          <t>BIELLMANN Cindy</t>
-        </is>
-      </c>
-    </row>
-    <row r="33"/>
+      <c r="G32" s="1" t="inlineStr">
+        <is>
+          <t>M 924</t>
+        </is>
+      </c>
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>ANDRZEJEWSKI Nicolas</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
+        <is>
+          <t>HIRSINGER Pascal</t>
+        </is>
+      </c>
+      <c r="J32" s="4" t="inlineStr">
+        <is>
+          <t>RUDLOFF Jérémy</t>
+        </is>
+      </c>
+      <c r="L32" s="3" t="inlineStr">
+        <is>
+          <t>SIMON Gael</t>
+        </is>
+      </c>
+      <c r="M32" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="H33" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="I33" s="3" t="inlineStr">
+        <is>
+          <t>HILDWEIN Steve</t>
+        </is>
+      </c>
+      <c r="J33" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+    </row>
     <row r="34">
-      <c r="G34" s="6" t="inlineStr">
-        <is>
-          <t>DA SILVA Axel</t>
+      <c r="L34" s="3" t="inlineStr">
+        <is>
+          <t>SCHREIBER Bertrand</t>
+        </is>
+      </c>
+      <c r="M34" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -882,32 +1125,78 @@
           <t>MANUTENTION LOURD</t>
         </is>
       </c>
-      <c r="C36" s="2" t="inlineStr">
+      <c r="C36" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOIREAU Stéphane </t>
+        </is>
+      </c>
+      <c r="D36" s="3" t="inlineStr">
         <is>
           <t>MOEGLING Vincent</t>
         </is>
       </c>
-      <c r="D36" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DJEBARA Philippe </t>
-        </is>
-      </c>
-      <c r="E36" s="3" t="inlineStr">
-        <is>
-          <t>MOSCOPOULOS Sébastien</t>
-        </is>
-      </c>
-      <c r="G36" s="6" t="inlineStr">
-        <is>
-          <t>DUCROT Déborah</t>
-        </is>
-      </c>
-    </row>
-    <row r="37"/>
+      <c r="E36" s="4" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
+        </is>
+      </c>
+      <c r="G36" s="1" t="inlineStr">
+        <is>
+          <t>M 718</t>
+        </is>
+      </c>
+      <c r="H36" s="2" t="inlineStr">
+        <is>
+          <t>MASSINON Frédéric</t>
+        </is>
+      </c>
+      <c r="I36" s="3" t="inlineStr">
+        <is>
+          <t>RAKOTONDRAMANANA Nivo</t>
+        </is>
+      </c>
+      <c r="J36" s="4" t="inlineStr">
+        <is>
+          <t>CORNOT David</t>
+        </is>
+      </c>
+      <c r="L36" s="3" t="inlineStr">
+        <is>
+          <t>BELIANE Karim</t>
+        </is>
+      </c>
+      <c r="M36" s="1" t="inlineStr">
+        <is>
+          <t>rtt</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="H37" s="2" t="inlineStr">
+        <is>
+          <t>PASQUIER Alexandre</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>ACKERMANN Rémy</t>
+        </is>
+      </c>
+      <c r="J37" s="4" t="inlineStr">
+        <is>
+          <t>ZWICKERT Xavier</t>
+        </is>
+      </c>
+    </row>
     <row r="38">
-      <c r="G38" s="6" t="inlineStr">
-        <is>
-          <t>GRIMONT Olivier</t>
+      <c r="L38" s="3" t="inlineStr">
+        <is>
+          <t>CAMACHO Michel</t>
+        </is>
+      </c>
+      <c r="M38" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -918,27 +1207,48 @@
           <t>2T</t>
         </is>
       </c>
-      <c r="C40" s="7" t="inlineStr">
+      <c r="C40" s="8" t="inlineStr">
         <is>
           <t>Vincent WENDLING</t>
         </is>
       </c>
-      <c r="E40" s="3" t="inlineStr">
-        <is>
-          <t>SCHENCK Emmanuel</t>
-        </is>
-      </c>
-      <c r="G40" s="6" t="inlineStr">
-        <is>
-          <t>GUMUS Fatih</t>
-        </is>
-      </c>
-    </row>
-    <row r="41"/>
+      <c r="G40" s="1" t="inlineStr">
+        <is>
+          <t>LMC</t>
+        </is>
+      </c>
+      <c r="H40" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L40" s="3" t="inlineStr">
+        <is>
+          <t>EBRAN Vincent</t>
+        </is>
+      </c>
+      <c r="M40" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="H41" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+    </row>
     <row r="42">
-      <c r="G42" s="6" t="inlineStr">
-        <is>
-          <t>HELFTER Franck</t>
+      <c r="L42" s="3" t="inlineStr">
+        <is>
+          <t>FONTAINE Fabien</t>
+        </is>
+      </c>
+      <c r="M42" s="1" t="inlineStr">
+        <is>
+          <t>rc</t>
         </is>
       </c>
     </row>
@@ -949,33 +1259,78 @@
           <t>M 1848/1</t>
         </is>
       </c>
-      <c r="C44" s="2" t="inlineStr">
+      <c r="D44" s="3" t="inlineStr">
         <is>
           <t>NETALA Frédéric</t>
         </is>
       </c>
-      <c r="G44" s="6" t="inlineStr">
-        <is>
-          <t>LICHTLE Jean-Sébastien</t>
+      <c r="E44" s="4" t="inlineStr">
+        <is>
+          <t>FRICKERT Florian</t>
+        </is>
+      </c>
+      <c r="G44" s="1" t="inlineStr">
+        <is>
+          <t>CENTRE-POSE</t>
+        </is>
+      </c>
+      <c r="H44" s="2" t="inlineStr">
+        <is>
+          <t>WEHRLEN Patrice</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>ROGLER Richard</t>
+        </is>
+      </c>
+      <c r="J44" s="4" t="inlineStr">
+        <is>
+          <t>KIEFFER Victor</t>
+        </is>
+      </c>
+      <c r="L44" s="3" t="inlineStr">
+        <is>
+          <t>HAIL Fehrat</t>
+        </is>
+      </c>
+      <c r="M44" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="C45" s="2" t="inlineStr">
+      <c r="D45" s="3" t="inlineStr">
         <is>
           <t>FRILLOT Jacky</t>
         </is>
       </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>SPITZ Eric</t>
+        </is>
+      </c>
     </row>
     <row r="46">
-      <c r="C46" s="2" t="inlineStr">
+      <c r="D46" s="3" t="inlineStr">
         <is>
           <t>HUGG Christian</t>
         </is>
       </c>
-      <c r="G46" s="6" t="inlineStr">
-        <is>
-          <t>ROUSSIN Frédéric</t>
+      <c r="E46" s="4" t="inlineStr">
+        <is>
+          <t>RENCKER Michel</t>
+        </is>
+      </c>
+      <c r="L46" s="3" t="inlineStr">
+        <is>
+          <t>ROSSE Madeline</t>
+        </is>
+      </c>
+      <c r="M46" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -988,27 +1343,62 @@
       </c>
       <c r="C48" s="2" t="inlineStr">
         <is>
+          <t>GRIMONT Olivier</t>
+        </is>
+      </c>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
           <t>FUCHS Eric</t>
         </is>
       </c>
-      <c r="E48" s="3" t="inlineStr">
-        <is>
-          <t>VILLEMIN Franck</t>
-        </is>
-      </c>
-      <c r="G48" s="6" t="inlineStr">
-        <is>
-          <t>SCANDELLA Christophe</t>
+      <c r="E48" s="4" t="inlineStr">
+        <is>
+          <t>GAVROY Gilles</t>
+        </is>
+      </c>
+      <c r="G48" s="1" t="inlineStr">
+        <is>
+          <t>ECOMAC</t>
+        </is>
+      </c>
+      <c r="H48" s="2" t="inlineStr">
+        <is>
+          <t>VIAUD Cyril</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>RIGOT Sébastien</t>
+        </is>
+      </c>
+      <c r="J48" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L48" s="2" t="inlineStr">
+        <is>
+          <t>BLATZ Jean-Marie</t>
+        </is>
+      </c>
+      <c r="M48" s="1" t="inlineStr">
+        <is>
+          <t>?</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="C49" s="2" t="inlineStr">
         <is>
-          <t>FONTAINE Fabien</t>
-        </is>
-      </c>
-      <c r="E49" s="3" t="inlineStr">
+          <t>DA SILVA Axel</t>
+        </is>
+      </c>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>AUDREN Olivier</t>
+        </is>
+      </c>
+      <c r="E49" s="4" t="inlineStr">
         <is>
           <t>DANIEL Jean-Luc</t>
         </is>
@@ -1017,17 +1407,27 @@
     <row r="50">
       <c r="C50" s="2" t="inlineStr">
         <is>
-          <t>AUDREN Olivier</t>
-        </is>
-      </c>
-      <c r="E50" s="3" t="inlineStr">
-        <is>
-          <t>FRICKERT Florian</t>
-        </is>
-      </c>
-      <c r="G50" s="6" t="inlineStr">
-        <is>
-          <t>SCHWARZ Jean-Philippe</t>
+          <t>SCANDELLA Christophe</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="E50" s="4" t="inlineStr">
+        <is>
+          <t>MOZET Gaétan</t>
+        </is>
+      </c>
+      <c r="L50" s="2" t="inlineStr">
+        <is>
+          <t>CORSET Christo</t>
+        </is>
+      </c>
+      <c r="M50" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -1038,28 +1438,63 @@
           <t>TCY</t>
         </is>
       </c>
-      <c r="E52" s="3" t="inlineStr">
-        <is>
-          <t>KIEFFER Victor</t>
-        </is>
-      </c>
-      <c r="G52" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PINTO José </t>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>SAHLI Halim</t>
+        </is>
+      </c>
+      <c r="G52" s="1" t="inlineStr">
+        <is>
+          <t>HST</t>
+        </is>
+      </c>
+      <c r="H52" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="I52" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L52" s="2" t="inlineStr">
+        <is>
+          <t>BIELLMANN Cindy</t>
+        </is>
+      </c>
+      <c r="M52" s="1" t="inlineStr">
+        <is>
+          <t>CP</t>
         </is>
       </c>
     </row>
     <row r="53">
-      <c r="E53" s="3" t="inlineStr">
-        <is>
-          <t>MOZET Gaétan</t>
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>FRITSCH Julien</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
         </is>
       </c>
     </row>
     <row r="54">
-      <c r="G54" s="3" t="inlineStr">
-        <is>
-          <t>DA COSTA Nelson</t>
+      <c r="L54" s="2" t="inlineStr">
+        <is>
+          <t>GIDEMANN Olivier</t>
+        </is>
+      </c>
+      <c r="M54" s="1" t="inlineStr">
+        <is>
+          <t>GE</t>
         </is>
       </c>
     </row>
@@ -1070,301 +1505,86 @@
           <t>SRE</t>
         </is>
       </c>
-      <c r="G56" s="3" t="inlineStr">
-        <is>
-          <t>FIGUEIREDO José</t>
+      <c r="L56" s="2" t="inlineStr">
+        <is>
+          <t>GUMUS Fatih</t>
+        </is>
+      </c>
+      <c r="M56" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="57"/>
     <row r="58">
-      <c r="G58" s="3" t="inlineStr">
-        <is>
-          <t>GAVROY Gilles</t>
+      <c r="L58" s="4" t="inlineStr">
+        <is>
+          <t>FIGUEIREDO José</t>
+        </is>
+      </c>
+      <c r="M58" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="59"/>
     <row r="60">
-      <c r="B60" s="1" t="inlineStr">
-        <is>
-          <t>SMT</t>
-        </is>
-      </c>
-      <c r="C60" s="2" t="inlineStr">
-        <is>
-          <t>BELIANE Karim</t>
-        </is>
-      </c>
-      <c r="G60" s="3" t="inlineStr">
-        <is>
-          <t>LOUIS Nicolas</t>
+      <c r="L60" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PISKA Laurent </t>
+        </is>
+      </c>
+      <c r="M60" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="61"/>
     <row r="62">
-      <c r="G62" s="3" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
+      <c r="L62" s="7" t="inlineStr">
+        <is>
+          <t>REIBEL Christophe</t>
+        </is>
+      </c>
+      <c r="M62" s="1" t="inlineStr">
+        <is>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="63"/>
     <row r="64">
-      <c r="B64" s="1" t="inlineStr">
-        <is>
-          <t>LBB1</t>
-        </is>
-      </c>
-      <c r="C64" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ROTH Mathieu </t>
-        </is>
-      </c>
-      <c r="G64" s="3" t="inlineStr">
-        <is>
-          <t>RUBIO Alexandre</t>
+      <c r="L64" s="2" t="inlineStr">
+        <is>
+          <t>LUDAESCHER Pascal</t>
+        </is>
+      </c>
+      <c r="M64" s="1" t="inlineStr">
+        <is>
+          <t>*</t>
         </is>
       </c>
     </row>
     <row r="65"/>
-    <row r="66">
-      <c r="G66" s="3" t="inlineStr">
-        <is>
-          <t>SPITZ Eric</t>
-        </is>
-      </c>
-    </row>
+    <row r="66"/>
     <row r="67"/>
-    <row r="68">
-      <c r="B68" s="1" t="inlineStr">
-        <is>
-          <t>MITRAILLEUSE</t>
-        </is>
-      </c>
-    </row>
+    <row r="68"/>
     <row r="69"/>
-    <row r="70"/>
+    <row r="70">
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Personnel non affecté</t>
+        </is>
+      </c>
+    </row>
     <row r="71"/>
     <row r="72">
-      <c r="B72" s="1" t="inlineStr">
-        <is>
-          <t>MITR. BIMAC</t>
-        </is>
-      </c>
-    </row>
-    <row r="73"/>
-    <row r="74"/>
-    <row r="75"/>
-    <row r="76">
-      <c r="B76" s="1" t="inlineStr">
-        <is>
-          <t>MANUTENTION INTÉGRÉ</t>
-        </is>
-      </c>
-      <c r="C76" s="2" t="inlineStr">
-        <is>
-          <t>RAMON Dominique</t>
-        </is>
-      </c>
-      <c r="D76" s="6" t="inlineStr">
-        <is>
-          <t>BAUMANN Mike</t>
-        </is>
-      </c>
-      <c r="E76" s="3" t="inlineStr">
-        <is>
-          <t>HOFFERT Patrick</t>
-        </is>
-      </c>
-    </row>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80">
-      <c r="B80" s="1" t="inlineStr">
-        <is>
-          <t>PRÉPARATEUR</t>
-        </is>
-      </c>
-      <c r="C80" s="2" t="inlineStr">
-        <is>
-          <t>CASPAR Gaël</t>
-        </is>
-      </c>
-      <c r="D80" s="6" t="inlineStr">
-        <is>
-          <t>HERMANN Cédric</t>
-        </is>
-      </c>
-      <c r="E80" s="3" t="inlineStr">
-        <is>
-          <t>RITT Jean Jacques</t>
-        </is>
-      </c>
-    </row>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84">
-      <c r="B84" s="1" t="inlineStr">
-        <is>
-          <t>M 1228</t>
-        </is>
-      </c>
-      <c r="C84" s="2" t="inlineStr">
-        <is>
-          <t>HAIL Fehrat</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="C85" s="3" t="inlineStr">
-        <is>
-          <t>GURLER Onur</t>
-        </is>
-      </c>
-    </row>
-    <row r="86"/>
-    <row r="87"/>
-    <row r="88">
-      <c r="B88" s="1" t="inlineStr">
-        <is>
-          <t>M 924</t>
-        </is>
-      </c>
-      <c r="C88" s="2" t="inlineStr">
-        <is>
-          <t>HIRSINGER Pascal</t>
-        </is>
-      </c>
-      <c r="E88" s="3" t="inlineStr">
-        <is>
-          <t>RUDLOFF Jérémy</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="C89" s="2" t="inlineStr">
-        <is>
-          <t>HILDWEIN Steve</t>
-        </is>
-      </c>
-      <c r="E89" s="3" t="inlineStr">
-        <is>
-          <t>CORNOT David</t>
-        </is>
-      </c>
-    </row>
-    <row r="90"/>
-    <row r="91"/>
-    <row r="92">
-      <c r="B92" s="1" t="inlineStr">
-        <is>
-          <t>M 718</t>
-        </is>
-      </c>
-      <c r="C92" s="2" t="inlineStr">
-        <is>
-          <t>RAKOTONDRAMANANA Nivo</t>
-        </is>
-      </c>
-      <c r="E92" s="3" t="inlineStr">
-        <is>
-          <t>FERDER Thomas</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="C93" s="3" t="inlineStr">
-        <is>
-          <t>LIER Romain</t>
-        </is>
-      </c>
-      <c r="E93" s="3" t="inlineStr">
-        <is>
-          <t>ZWICKERT Xavier</t>
-        </is>
-      </c>
-    </row>
-    <row r="94"/>
-    <row r="95"/>
-    <row r="96">
-      <c r="B96" s="1" t="inlineStr">
-        <is>
-          <t>LMC</t>
-        </is>
-      </c>
-      <c r="C96" s="2" t="inlineStr">
-        <is>
-          <t>EBRAN Vincent</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="C97" s="2" t="inlineStr">
-        <is>
-          <t>ROSSE Madeline</t>
-        </is>
-      </c>
-    </row>
-    <row r="98"/>
-    <row r="99"/>
-    <row r="100">
-      <c r="B100" s="1" t="inlineStr">
-        <is>
-          <t>CENTRE-POSE</t>
-        </is>
-      </c>
-      <c r="C100" s="6" t="inlineStr">
-        <is>
-          <t>GRASSIN Axel</t>
-        </is>
-      </c>
-      <c r="D100" s="6" t="inlineStr">
-        <is>
-          <t>WEHRLEN Patrice</t>
-        </is>
-      </c>
-      <c r="E100" s="3" t="inlineStr">
-        <is>
-          <t>TRAPANESE Antoine</t>
-        </is>
-      </c>
-    </row>
-    <row r="101"/>
-    <row r="102"/>
-    <row r="103"/>
-    <row r="104">
-      <c r="B104" s="1" t="inlineStr">
-        <is>
-          <t>ECOMAC</t>
-        </is>
-      </c>
-      <c r="C104" s="2" t="inlineStr">
-        <is>
-          <t>RIGOT Sébastien</t>
-        </is>
-      </c>
-      <c r="D104" s="6" t="inlineStr">
-        <is>
-          <t>VIAUD Cyril</t>
-        </is>
-      </c>
-    </row>
-    <row r="105"/>
-    <row r="106"/>
-    <row r="107"/>
-    <row r="108">
-      <c r="B108" s="1" t="inlineStr">
-        <is>
-          <t>HST</t>
-        </is>
-      </c>
-      <c r="C108" s="8" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="L72" s="4" t="inlineStr">
+        <is>
+          <t>RUBIO Alexandre</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
petite modif excel + ajout des contremaîtres
</commit_message>
<xml_diff>
--- a/planning/static/excel/planning.xlsx
+++ b/planning/static/excel/planning.xlsx
@@ -47,6 +47,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFBF00"/>
         <bgColor rgb="FFFFBF00"/>
       </patternFill>
@@ -61,12 +67,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF6D6D"/>
         <bgColor rgb="FFFF6D6D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor rgb="FF99FF99"/>
       </patternFill>
     </fill>
     <fill>
@@ -106,12 +106,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -558,22 +558,22 @@
     <row r="4">
       <c r="B4" s="1" t="inlineStr">
         <is>
-          <t>B 1604</t>
+          <t>CONTREMAÎTRES</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>HELFTER Franck</t>
+          <t>SIMLER Maurice</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>VINGATARAMIN Pierre</t>
+          <t>FRITSCH Patrick</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>BROGLIE Julien</t>
+          <t>DEPARIS Frédéric</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
@@ -603,38 +603,23 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>SCHILLINGER  Jérémy</t>
+      <c r="C5" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>HORACEK Julien</t>
-        </is>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+          <t>WENDLING Christophe</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>PISKA Laurent</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>CAMARASA Sébastien</t>
-        </is>
-      </c>
-      <c r="D6" s="3" t="inlineStr">
-        <is>
-          <t>HUEBER Olivier</t>
-        </is>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
       <c r="L6" s="4" t="inlineStr">
         <is>
           <t>FULLERINGER Gaétan</t>
@@ -650,22 +635,22 @@
     <row r="8">
       <c r="B8" s="1" t="inlineStr">
         <is>
-          <t>B 2100</t>
+          <t>B 1604</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>DUCROT Déborah</t>
+          <t>HELFTER Franck</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
         <is>
-          <t>LUDAESCHER Olivier</t>
+          <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
       <c r="E8" s="4" t="inlineStr">
         <is>
-          <t>MORENO José</t>
+          <t>BROGLIE Julien</t>
         </is>
       </c>
       <c r="G8" s="1" t="inlineStr">
@@ -687,34 +672,34 @@
     <row r="9">
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>ROUSSIN Frédéric</t>
+          <t>SCHILLINGER  Jérémy</t>
         </is>
       </c>
       <c r="D9" s="3" t="inlineStr">
         <is>
-          <t>HAAG Patrick</t>
-        </is>
-      </c>
-      <c r="E9" s="4" t="inlineStr">
-        <is>
-          <t>ABELLAN GRINAN Laurent</t>
+          <t>HORACEK Julien</t>
+        </is>
+      </c>
+      <c r="E9" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>LICHTLE Jean-Sébastien</t>
-        </is>
-      </c>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
-        </is>
-      </c>
-      <c r="E10" s="4" t="inlineStr">
-        <is>
-          <t>SCHAAL Eric</t>
+          <t>CAMARASA Sébastien</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>HUEBER Olivier</t>
+        </is>
+      </c>
+      <c r="E10" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="L10" s="4" t="inlineStr">
@@ -732,12 +717,22 @@
     <row r="12">
       <c r="B12" s="1" t="inlineStr">
         <is>
-          <t>B2000</t>
+          <t>B 2100</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>DUCROT Déborah</t>
         </is>
       </c>
       <c r="D12" s="3" t="inlineStr">
         <is>
-          <t>SIGWALT Thierry</t>
+          <t>LUDAESCHER Olivier</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>MORENO José</t>
         </is>
       </c>
       <c r="G12" s="1" t="inlineStr">
@@ -762,13 +757,38 @@
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>NESZCZADYN Franck</t>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>ROUSSIN Frédéric</t>
+        </is>
+      </c>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>HAAG Patrick</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>ABELLAN GRINAN Laurent</t>
         </is>
       </c>
     </row>
     <row r="14">
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>LICHTLE Jean-Sébastien</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>CASPAR Gaël</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>SCHAAL Eric</t>
+        </is>
+      </c>
       <c r="L14" s="4" t="inlineStr">
         <is>
           <t>TRAPANESE Antoine</t>
@@ -784,17 +804,12 @@
     <row r="16">
       <c r="B16" s="1" t="inlineStr">
         <is>
-          <t>G 1628</t>
-        </is>
-      </c>
-      <c r="D16" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="E16" s="4" t="inlineStr">
-        <is>
-          <t>FOECHTERLE Jean</t>
+          <t>B2000</t>
+        </is>
+      </c>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>SIGWALT Thierry</t>
         </is>
       </c>
       <c r="G16" s="1" t="inlineStr">
@@ -814,28 +829,13 @@
       </c>
     </row>
     <row r="17">
-      <c r="D17" s="3" t="inlineStr">
-        <is>
-          <t>GEIGER Frédéric</t>
-        </is>
-      </c>
-      <c r="E17" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>NESZCZADYN Franck</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
-        </is>
-      </c>
-      <c r="E18" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
       <c r="L18" s="4" t="inlineStr">
         <is>
           <t>YEGEN Zulkifar</t>
@@ -851,22 +851,17 @@
     <row r="20">
       <c r="B20" s="1" t="inlineStr">
         <is>
-          <t>DOMINO</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>BERGER Virgil</t>
-        </is>
-      </c>
-      <c r="D20" s="3" t="inlineStr">
-        <is>
-          <t>BAUMANN Dylan</t>
-        </is>
-      </c>
-      <c r="E20" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
+          <t>G 1628</t>
+        </is>
+      </c>
+      <c r="D20" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>FOECHTERLE Jean</t>
         </is>
       </c>
       <c r="G20" s="1" t="inlineStr">
@@ -900,8 +895,29 @@
         </is>
       </c>
     </row>
-    <row r="21"/>
+    <row r="21">
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>GEIGER Frédéric</t>
+        </is>
+      </c>
+      <c r="E21" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+    </row>
     <row r="22">
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="E22" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
       <c r="L22" s="4" t="inlineStr">
         <is>
           <t>FERDER Thomas</t>
@@ -917,42 +933,42 @@
     <row r="24">
       <c r="B24" s="1" t="inlineStr">
         <is>
-          <t>PRESSE À BALLE</t>
-        </is>
-      </c>
-      <c r="C24" s="6" t="inlineStr">
+          <t>DOMINO</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>BERGER Virgil</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>BAUMANN Dylan</t>
+        </is>
+      </c>
+      <c r="E24" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KOESSEL Marc </t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>PRÉPARATEUR</t>
+        </is>
+      </c>
+      <c r="H24" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="D24" s="6" t="inlineStr">
+      <c r="I24" s="6" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
-        <is>
-          <t>MULLER Gilbert</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>PRÉPARATEUR</t>
-        </is>
-      </c>
-      <c r="H24" s="2" t="inlineStr">
-        <is>
-          <t>HERMANN Cédric</t>
-        </is>
-      </c>
-      <c r="I24" s="3" t="inlineStr">
-        <is>
-          <t>CASPAR Gaël</t>
-        </is>
-      </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>RITT Jean Jacques</t>
+      <c r="J24" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="L24" s="7" t="inlineStr">
@@ -983,7 +999,22 @@
     <row r="28">
       <c r="B28" s="1" t="inlineStr">
         <is>
-          <t>PLATEAUX</t>
+          <t>PRESSE À BALLE</t>
+        </is>
+      </c>
+      <c r="C28" s="4" t="inlineStr">
+        <is>
+          <t>RITT Jean Jacques</t>
+        </is>
+      </c>
+      <c r="D28" s="6" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E28" s="4" t="inlineStr">
+        <is>
+          <t>MULLER Gilbert</t>
         </is>
       </c>
       <c r="G28" s="1" t="inlineStr">
@@ -1040,22 +1071,7 @@
     <row r="32">
       <c r="B32" s="1" t="inlineStr">
         <is>
-          <t>EMBALLAGE</t>
-        </is>
-      </c>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>LEROY Nicolas</t>
-        </is>
-      </c>
-      <c r="D32" s="3" t="inlineStr">
-        <is>
-          <t>SUTTER Thierry</t>
-        </is>
-      </c>
-      <c r="E32" s="4" t="inlineStr">
-        <is>
-          <t>GANTNER Stéphane</t>
+          <t>PLATEAUX</t>
         </is>
       </c>
       <c r="G32" s="1" t="inlineStr">
@@ -1090,9 +1106,9 @@
       </c>
     </row>
     <row r="33">
-      <c r="H33" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+      <c r="H33" s="2" t="inlineStr">
+        <is>
+          <t>HERMANN Cédric</t>
         </is>
       </c>
       <c r="I33" s="3" t="inlineStr">
@@ -1122,22 +1138,22 @@
     <row r="36">
       <c r="B36" s="1" t="inlineStr">
         <is>
-          <t>MANUTENTION LOURD</t>
-        </is>
-      </c>
-      <c r="C36" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BOIREAU Stéphane </t>
+          <t>EMBALLAGE</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>LEROY Nicolas</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>MOEGLING Vincent</t>
+          <t>SUTTER Thierry</t>
         </is>
       </c>
       <c r="E36" s="4" t="inlineStr">
         <is>
-          <t>SCHENCK Emmanuel</t>
+          <t>GANTNER Stéphane</t>
         </is>
       </c>
       <c r="G36" s="1" t="inlineStr">
@@ -1204,12 +1220,22 @@
     <row r="40">
       <c r="B40" s="1" t="inlineStr">
         <is>
-          <t>2T</t>
-        </is>
-      </c>
-      <c r="C40" s="8" t="inlineStr">
-        <is>
-          <t>Vincent WENDLING</t>
+          <t>MANUTENTION LOURD</t>
+        </is>
+      </c>
+      <c r="C40" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BOIREAU Stéphane </t>
+        </is>
+      </c>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>MOEGLING Vincent</t>
+        </is>
+      </c>
+      <c r="E40" s="4" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
         </is>
       </c>
       <c r="G40" s="1" t="inlineStr">
@@ -1256,17 +1282,12 @@
     <row r="44">
       <c r="B44" s="1" t="inlineStr">
         <is>
-          <t>M 1848/1</t>
-        </is>
-      </c>
-      <c r="D44" s="3" t="inlineStr">
-        <is>
-          <t>NETALA Frédéric</t>
-        </is>
-      </c>
-      <c r="E44" s="4" t="inlineStr">
-        <is>
-          <t>FRICKERT Florian</t>
+          <t>2T</t>
+        </is>
+      </c>
+      <c r="C44" s="8" t="inlineStr">
+        <is>
+          <t>Vincent WENDLING</t>
         </is>
       </c>
       <c r="G44" s="1" t="inlineStr">
@@ -1300,29 +1321,8 @@
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="D45" s="3" t="inlineStr">
-        <is>
-          <t>FRILLOT Jacky</t>
-        </is>
-      </c>
-      <c r="E45" s="4" t="inlineStr">
-        <is>
-          <t>SPITZ Eric</t>
-        </is>
-      </c>
-    </row>
+    <row r="45"/>
     <row r="46">
-      <c r="D46" s="3" t="inlineStr">
-        <is>
-          <t>HUGG Christian</t>
-        </is>
-      </c>
-      <c r="E46" s="4" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
-        </is>
-      </c>
       <c r="L46" s="3" t="inlineStr">
         <is>
           <t>ROSSE Madeline</t>
@@ -1338,22 +1338,17 @@
     <row r="48">
       <c r="B48" s="1" t="inlineStr">
         <is>
-          <t>M 1848/2</t>
-        </is>
-      </c>
-      <c r="C48" s="2" t="inlineStr">
-        <is>
-          <t>GRIMONT Olivier</t>
+          <t>M 1848/1</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>FUCHS Eric</t>
+          <t>NETALA Frédéric</t>
         </is>
       </c>
       <c r="E48" s="4" t="inlineStr">
         <is>
-          <t>GAVROY Gilles</t>
+          <t>FRICKERT Florian</t>
         </is>
       </c>
       <c r="G48" s="1" t="inlineStr">
@@ -1388,36 +1383,26 @@
       </c>
     </row>
     <row r="49">
-      <c r="C49" s="2" t="inlineStr">
-        <is>
-          <t>DA SILVA Axel</t>
-        </is>
-      </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>AUDREN Olivier</t>
+          <t>FRILLOT Jacky</t>
         </is>
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>DANIEL Jean-Luc</t>
+          <t>SPITZ Eric</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="C50" s="2" t="inlineStr">
-        <is>
-          <t>SCANDELLA Christophe</t>
-        </is>
-      </c>
-      <c r="D50" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
+      <c r="D50" s="3" t="inlineStr">
+        <is>
+          <t>HUGG Christian</t>
         </is>
       </c>
       <c r="E50" s="4" t="inlineStr">
         <is>
-          <t>MOZET Gaétan</t>
+          <t>RENCKER Michel</t>
         </is>
       </c>
       <c r="L50" s="2" t="inlineStr">
@@ -1435,17 +1420,22 @@
     <row r="52">
       <c r="B52" s="1" t="inlineStr">
         <is>
-          <t>TCY</t>
+          <t>M 1848/2</t>
         </is>
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
-          <t>SCHWARZ Jean-Philippe</t>
+          <t>GRIMONT Olivier</t>
         </is>
       </c>
       <c r="D52" s="3" t="inlineStr">
         <is>
-          <t>SAHLI Halim</t>
+          <t>FUCHS Eric</t>
+        </is>
+      </c>
+      <c r="E52" s="4" t="inlineStr">
+        <is>
+          <t>GAVROY Gilles</t>
         </is>
       </c>
       <c r="G52" s="1" t="inlineStr">
@@ -1477,16 +1467,36 @@
     <row r="53">
       <c r="C53" s="2" t="inlineStr">
         <is>
-          <t>FRITSCH Julien</t>
+          <t>DA SILVA Axel</t>
         </is>
       </c>
       <c r="D53" s="3" t="inlineStr">
         <is>
-          <t>LEDER Frédéric</t>
+          <t>AUDREN Olivier</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
+        <is>
+          <t>DANIEL Jean-Luc</t>
         </is>
       </c>
     </row>
     <row r="54">
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>SCANDELLA Christophe</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="E54" s="4" t="inlineStr">
+        <is>
+          <t>MOZET Gaétan</t>
+        </is>
+      </c>
       <c r="L54" s="2" t="inlineStr">
         <is>
           <t>GIDEMANN Olivier</t>
@@ -1502,7 +1512,17 @@
     <row r="56">
       <c r="B56" s="1" t="inlineStr">
         <is>
-          <t>SRE</t>
+          <t>TCY</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
+        </is>
+      </c>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>SAHLI Halim</t>
         </is>
       </c>
       <c r="L56" s="2" t="inlineStr">
@@ -1516,7 +1536,18 @@
         </is>
       </c>
     </row>
-    <row r="57"/>
+    <row r="57">
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>FRITSCH Julien</t>
+        </is>
+      </c>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
+        </is>
+      </c>
+    </row>
     <row r="58">
       <c r="L58" s="4" t="inlineStr">
         <is>
@@ -1531,6 +1562,11 @@
     </row>
     <row r="59"/>
     <row r="60">
+      <c r="B60" s="1" t="inlineStr">
+        <is>
+          <t>SRE</t>
+        </is>
+      </c>
       <c r="L60" s="7" t="inlineStr">
         <is>
           <t xml:space="preserve">PISKA Laurent </t>
@@ -1544,7 +1580,7 @@
     </row>
     <row r="61"/>
     <row r="62">
-      <c r="L62" s="7" t="inlineStr">
+      <c r="L62" s="2" t="inlineStr">
         <is>
           <t>REIBEL Christophe</t>
         </is>

</xml_diff>

<commit_message>
bug couleur intérimaire dans le fichier excel
</commit_message>
<xml_diff>
--- a/planning/static/excel/planning.xlsx
+++ b/planning/static/excel/planning.xlsx
@@ -35,6 +35,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor rgb="FF99FF99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFFBF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
@@ -47,24 +59,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF99"/>
-        <bgColor rgb="FF99FF99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFBF00"/>
-        <bgColor rgb="FFFFBF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF6D6D"/>
         <bgColor rgb="FFFF6D6D"/>
       </patternFill>
@@ -73,6 +67,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -106,12 +106,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,11 +488,11 @@
     <col customWidth="1" max="1" min="1" width="14.4"/>
     <col customWidth="1" max="2" min="2" width="22.8"/>
     <col customWidth="1" max="3" min="3" width="28.8"/>
-    <col customWidth="1" max="4" min="4" width="25.2"/>
-    <col customWidth="1" max="5" min="5" width="28.8"/>
+    <col customWidth="1" max="4" min="4" width="28.8"/>
+    <col customWidth="1" max="5" min="5" width="25.2"/>
     <col customWidth="1" max="6" min="6" width="7.199999999999999"/>
     <col customWidth="1" max="7" min="7" width="25.2"/>
-    <col customWidth="1" max="8" min="8" width="26.4"/>
+    <col customWidth="1" max="8" min="8" width="22.8"/>
     <col customWidth="1" max="9" min="9" width="27.6"/>
     <col customWidth="1" max="10" min="10" width="22.8"/>
     <col customWidth="1" max="11" min="11" width="7.199999999999999"/>
@@ -503,14 +503,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Semaine 19</t>
+          <t>Semaine 18</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MERCREDI</t>
+          <t>LUNDI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -563,35 +563,30 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>SIMLER Maurice</t>
+          <t>DEPARIS Frédéric</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>FRITSCH Patrick</t>
+          <t>REIBEL Christophe</t>
         </is>
       </c>
       <c r="E4" s="4" t="inlineStr">
         <is>
-          <t>DEPARIS Frédéric</t>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
-          <t>SMT</t>
-        </is>
-      </c>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ROTH Mathieu </t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DJEBARA Philippe </t>
-        </is>
-      </c>
-      <c r="L4" s="4" t="inlineStr">
+          <t>SRE</t>
+        </is>
+      </c>
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>DA COSTA Nelson</t>
         </is>
@@ -603,26 +598,26 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>PISKA Laurent</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>WENDLING Christophe</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>PISKA Laurent</t>
-        </is>
-      </c>
     </row>
     <row r="6">
-      <c r="L6" s="4" t="inlineStr">
-        <is>
-          <t>FULLERINGER Gaétan</t>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>LOUIS Nicolas</t>
         </is>
       </c>
       <c r="M6" s="1" t="inlineStr">
@@ -640,76 +635,86 @@
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
+          <t>BROGLIE Julien</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
           <t>HELFTER Franck</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>BROGLIE Julien</t>
-        </is>
-      </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
-          <t>LBB1</t>
-        </is>
-      </c>
-      <c r="L8" s="4" t="inlineStr">
-        <is>
-          <t>LOUIS Nicolas</t>
+          <t>SMT</t>
+        </is>
+      </c>
+      <c r="H8" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DJEBARA Philippe </t>
+        </is>
+      </c>
+      <c r="I8" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>YEGEN Zulkifar</t>
         </is>
       </c>
       <c r="M8" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="2" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>SCHILLINGER  Jérémy</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>HORACEK Julien</t>
         </is>
       </c>
-      <c r="E9" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
     </row>
     <row r="10">
-      <c r="C10" s="2" t="inlineStr">
+      <c r="C10" s="3" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>CAMARASA Sébastien</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>HUEBER Olivier</t>
         </is>
       </c>
-      <c r="E10" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L10" s="4" t="inlineStr">
-        <is>
-          <t>MOSCOPOULOS Sébastien</t>
+      <c r="L10" s="7" t="inlineStr">
+        <is>
+          <t>DA SILVA David</t>
         </is>
       </c>
       <c r="M10" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -722,32 +727,27 @@
       </c>
       <c r="C12" s="2" t="inlineStr">
         <is>
+          <t>MORENO José</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
           <t>DUCROT Déborah</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>LUDAESCHER Olivier</t>
         </is>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>MORENO José</t>
-        </is>
-      </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
-          <t>MITRAILLEUSE</t>
-        </is>
-      </c>
-      <c r="I12" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PINTO José </t>
-        </is>
-      </c>
-      <c r="L12" s="4" t="inlineStr">
-        <is>
-          <t>SPIELMANN Patrice</t>
+          <t>LBB1</t>
+        </is>
+      </c>
+      <c r="L12" s="5" t="inlineStr">
+        <is>
+          <t>BAUMANN Dylan</t>
         </is>
       </c>
       <c r="M12" s="1" t="inlineStr">
@@ -759,44 +759,44 @@
     <row r="13">
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>ROUSSIN Frédéric</t>
+          <t>ABELLAN GRINAN Laurent</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
+          <t>LUDAESCHER Pascal</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
           <t>HAAG Patrick</t>
-        </is>
-      </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>ABELLAN GRINAN Laurent</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>LICHTLE Jean-Sébastien</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
+          <t>SCHAAL Eric</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KOESSEL Marc </t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
         <is>
           <t>CASPAR Gaël</t>
         </is>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>SCHAAL Eric</t>
-        </is>
-      </c>
-      <c r="L14" s="4" t="inlineStr">
-        <is>
-          <t>TRAPANESE Antoine</t>
+      <c r="L14" s="5" t="inlineStr">
+        <is>
+          <t>ACKERMANN Rémy</t>
         </is>
       </c>
       <c r="M14" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>am</t>
         </is>
       </c>
     </row>
@@ -807,43 +807,58 @@
           <t>B2000</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>RUBIO Alexandre</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>SIGWALT Thierry</t>
         </is>
       </c>
       <c r="G16" s="1" t="inlineStr">
         <is>
-          <t>MITR. BIMAC</t>
-        </is>
-      </c>
-      <c r="L16" s="4" t="inlineStr">
+          <t>MITRAILLEUSE</t>
+        </is>
+      </c>
+      <c r="H16" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PINTO José </t>
+        </is>
+      </c>
+      <c r="L16" s="5" t="inlineStr">
+        <is>
+          <t>AUDREN Olivier</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>WITZ Alain</t>
         </is>
       </c>
-      <c r="M16" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>NESZCZADYN Franck</t>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>SIMON Gael</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="L18" s="4" t="inlineStr">
-        <is>
-          <t>YEGEN Zulkifar</t>
+      <c r="L18" s="5" t="inlineStr">
+        <is>
+          <t>BELIANE Karim</t>
         </is>
       </c>
       <c r="M18" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -854,39 +869,29 @@
           <t>G 1628</t>
         </is>
       </c>
-      <c r="D20" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>FOECHTERLE Jean</t>
         </is>
       </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>NESZCZADYN Franck</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>BUCHER Cyril</t>
+        </is>
+      </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
-          <t>MANUTENTION INTÉGRÉ</t>
-        </is>
-      </c>
-      <c r="H20" s="2" t="inlineStr">
-        <is>
-          <t>BAUMANN Mike</t>
-        </is>
-      </c>
-      <c r="I20" s="3" t="inlineStr">
-        <is>
-          <t>RAMON Dominique</t>
-        </is>
-      </c>
-      <c r="J20" s="4" t="inlineStr">
-        <is>
-          <t>HOFFERT Patrick</t>
-        </is>
-      </c>
-      <c r="L20" s="7" t="inlineStr">
-        <is>
-          <t>DA SILVA David</t>
+          <t>MITR. BIMAC</t>
+        </is>
+      </c>
+      <c r="L20" s="5" t="inlineStr">
+        <is>
+          <t>EBRAN Vincent</t>
         </is>
       </c>
       <c r="M20" s="1" t="inlineStr">
@@ -896,36 +901,46 @@
       </c>
     </row>
     <row r="21">
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>FULLERINGER Gaétan</t>
+        </is>
+      </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
+          <t>BLATZ Jean-Marie</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
           <t>GEIGER Frédéric</t>
         </is>
       </c>
-      <c r="E21" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
     </row>
     <row r="22">
-      <c r="D22" s="2" t="inlineStr">
+      <c r="C22" s="3" t="inlineStr">
         <is>
           <t>Intérimaire</t>
         </is>
       </c>
-      <c r="E22" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>FERDER Thomas</t>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>LICHTLE Jean-Sébastien</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t>SAHLI Halim</t>
+        </is>
+      </c>
+      <c r="L22" s="5" t="inlineStr">
+        <is>
+          <t>HAIL Fehrat</t>
         </is>
       </c>
       <c r="M22" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -938,60 +953,60 @@
       </c>
       <c r="C24" s="2" t="inlineStr">
         <is>
+          <t>SPIELMANN Patrice</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
           <t>BERGER Virgil</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>BAUMANN Dylan</t>
-        </is>
-      </c>
-      <c r="E24" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="G24" s="1" t="inlineStr">
         <is>
-          <t>PRÉPARATEUR</t>
-        </is>
-      </c>
-      <c r="H24" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="I24" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="J24" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L24" s="7" t="inlineStr">
-        <is>
-          <t>GURLER ONUR</t>
+          <t>MANUTENTION INTÉGRÉ</t>
+        </is>
+      </c>
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>HOFFERT Patrick</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
+        <is>
+          <t>BAUMANN Mike</t>
+        </is>
+      </c>
+      <c r="J24" s="5" t="inlineStr">
+        <is>
+          <t>RAMON Dominique</t>
+        </is>
+      </c>
+      <c r="L24" s="5" t="inlineStr">
+        <is>
+          <t>HIRSINGER Pascal</t>
         </is>
       </c>
       <c r="M24" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>rc</t>
         </is>
       </c>
     </row>
     <row r="25"/>
     <row r="26">
-      <c r="L26" s="4" t="inlineStr">
-        <is>
-          <t>LIER Romain</t>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>NETALA Frédéric</t>
         </is>
       </c>
       <c r="M26" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>rtt</t>
         </is>
       </c>
     </row>
@@ -1002,68 +1017,62 @@
           <t>PRESSE À BALLE</t>
         </is>
       </c>
-      <c r="C28" s="4" t="inlineStr">
-        <is>
-          <t>RITT Jean Jacques</t>
-        </is>
-      </c>
-      <c r="D28" s="6" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>MULLER Gilbert</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>RAKOTONDRAMANANA Nivo</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>SCHREIBER Bertrand</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>PRÉPARATEUR</t>
+        </is>
+      </c>
+      <c r="H28" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>MULLER Gilbert</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="inlineStr">
-        <is>
-          <t>M 1228</t>
-        </is>
-      </c>
-      <c r="H28" s="2" t="inlineStr">
-        <is>
-          <t>GRASSIN Axel</t>
+      <c r="I28" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="J28" s="4" t="inlineStr">
         <is>
-          <t>FRICKERT Rémy</t>
-        </is>
-      </c>
-      <c r="L28" s="4" t="inlineStr">
-        <is>
-          <t>VILLEMIN Franck</t>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>ROGLER Richard</t>
         </is>
       </c>
       <c r="M28" s="1" t="inlineStr">
         <is>
-          <t>C</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="H29" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="J29" s="4" t="inlineStr">
-        <is>
-          <t>GURLER Onur</t>
-        </is>
-      </c>
-    </row>
+          <t>D</t>
+        </is>
+      </c>
+    </row>
+    <row r="29"/>
     <row r="30">
       <c r="L30" s="3" t="inlineStr">
         <is>
-          <t>BUCHER Cyril</t>
+          <t>CORSET Christo</t>
         </is>
       </c>
       <c r="M30" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -1076,47 +1085,37 @@
       </c>
       <c r="G32" s="1" t="inlineStr">
         <is>
-          <t>M 924</t>
+          <t>M 1228</t>
         </is>
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>ANDRZEJEWSKI Nicolas</t>
+          <t>FRICKERT Rémy</t>
         </is>
       </c>
       <c r="I32" s="3" t="inlineStr">
         <is>
-          <t>HIRSINGER Pascal</t>
-        </is>
-      </c>
-      <c r="J32" s="4" t="inlineStr">
-        <is>
-          <t>RUDLOFF Jérémy</t>
+          <t>GRASSIN Axel</t>
         </is>
       </c>
       <c r="L32" s="3" t="inlineStr">
         <is>
-          <t>SIMON Gael</t>
+          <t>LEROY Nicolas</t>
         </is>
       </c>
       <c r="M32" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>HERMANN Cédric</t>
-        </is>
-      </c>
-      <c r="I33" s="3" t="inlineStr">
-        <is>
-          <t>HILDWEIN Steve</t>
-        </is>
-      </c>
-      <c r="J33" s="6" t="inlineStr">
+          <t>GURLER Onur</t>
+        </is>
+      </c>
+      <c r="I33" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
@@ -1125,7 +1124,7 @@
     <row r="34">
       <c r="L34" s="3" t="inlineStr">
         <is>
-          <t>SCHREIBER Bertrand</t>
+          <t>ROUSSIN Frédéric</t>
         </is>
       </c>
       <c r="M34" s="1" t="inlineStr">
@@ -1143,71 +1142,71 @@
       </c>
       <c r="C36" s="2" t="inlineStr">
         <is>
-          <t>LEROY Nicolas</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="inlineStr">
+          <t>GANTNER Stéphane</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ROTH Mathieu </t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="inlineStr">
         <is>
           <t>SUTTER Thierry</t>
         </is>
       </c>
-      <c r="E36" s="4" t="inlineStr">
-        <is>
-          <t>GANTNER Stéphane</t>
-        </is>
-      </c>
       <c r="G36" s="1" t="inlineStr">
         <is>
-          <t>M 718</t>
+          <t>M 924</t>
         </is>
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>MASSINON Frédéric</t>
-        </is>
-      </c>
-      <c r="I36" s="3" t="inlineStr">
-        <is>
-          <t>RAKOTONDRAMANANA Nivo</t>
-        </is>
-      </c>
-      <c r="J36" s="4" t="inlineStr">
-        <is>
-          <t>CORNOT David</t>
-        </is>
-      </c>
-      <c r="L36" s="3" t="inlineStr">
-        <is>
-          <t>BELIANE Karim</t>
+          <t>RUDLOFF Jérémy</t>
+        </is>
+      </c>
+      <c r="I36" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="J36" s="5" t="inlineStr">
+        <is>
+          <t>HILDWEIN Steve</t>
+        </is>
+      </c>
+      <c r="L36" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHULER Evelyne </t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>rtt</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="H37" s="2" t="inlineStr">
-        <is>
-          <t>PASQUIER Alexandre</t>
-        </is>
-      </c>
-      <c r="I37" s="3" t="inlineStr">
-        <is>
-          <t>ACKERMANN Rémy</t>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>HERMANN Cédric</t>
+        </is>
+      </c>
+      <c r="I37" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="J37" s="4" t="inlineStr">
         <is>
-          <t>ZWICKERT Xavier</t>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="L38" s="3" t="inlineStr">
         <is>
-          <t>CAMACHO Michel</t>
+          <t>ANDRZEJEWSKI Nicolas</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
@@ -1223,44 +1222,54 @@
           <t>MANUTENTION LOURD</t>
         </is>
       </c>
-      <c r="C40" s="5" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>MOSCOPOULOS Sébastien</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">BOIREAU Stéphane </t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
+      <c r="E40" s="5" t="inlineStr">
         <is>
           <t>MOEGLING Vincent</t>
         </is>
       </c>
-      <c r="E40" s="4" t="inlineStr">
-        <is>
-          <t>SCHENCK Emmanuel</t>
-        </is>
-      </c>
       <c r="G40" s="1" t="inlineStr">
         <is>
-          <t>LMC</t>
-        </is>
-      </c>
-      <c r="H40" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
+          <t>M 718</t>
+        </is>
+      </c>
+      <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>FERDER Thomas</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>MASSINON Frédéric</t>
         </is>
       </c>
       <c r="L40" s="3" t="inlineStr">
         <is>
-          <t>EBRAN Vincent</t>
+          <t>BIELLMANN Cindy</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>CP</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="H41" s="6" t="inlineStr">
+      <c r="H41" s="2" t="inlineStr">
+        <is>
+          <t>ZWICKERT Xavier</t>
+        </is>
+      </c>
+      <c r="I41" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
@@ -1269,12 +1278,12 @@
     <row r="42">
       <c r="L42" s="3" t="inlineStr">
         <is>
-          <t>FONTAINE Fabien</t>
+          <t>FRITSCH Julien</t>
         </is>
       </c>
       <c r="M42" s="1" t="inlineStr">
         <is>
-          <t>rc</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1285,52 +1294,58 @@
           <t>2T</t>
         </is>
       </c>
-      <c r="C44" s="8" t="inlineStr">
-        <is>
-          <t>Vincent WENDLING</t>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
         </is>
       </c>
       <c r="G44" s="1" t="inlineStr">
         <is>
-          <t>CENTRE-POSE</t>
+          <t>LMC</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>WEHRLEN Patrice</t>
-        </is>
-      </c>
-      <c r="I44" s="3" t="inlineStr">
-        <is>
-          <t>ROGLER Richard</t>
-        </is>
-      </c>
-      <c r="J44" s="4" t="inlineStr">
-        <is>
-          <t>KIEFFER Victor</t>
+          <t>CORNOT David</t>
+        </is>
+      </c>
+      <c r="J44" s="5" t="inlineStr">
+        <is>
+          <t>CAMACHO Michel</t>
         </is>
       </c>
       <c r="L44" s="3" t="inlineStr">
         <is>
-          <t>HAIL Fehrat</t>
+          <t>GIDEMANN Olivier</t>
         </is>
       </c>
       <c r="M44" s="1" t="inlineStr">
         <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
-    <row r="45"/>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="H45" s="2" t="inlineStr">
+        <is>
+          <t>LIER Romain</t>
+        </is>
+      </c>
+      <c r="J45" s="5" t="inlineStr">
+        <is>
+          <t>ROSSE Madeline</t>
+        </is>
+      </c>
+    </row>
     <row r="46">
       <c r="L46" s="3" t="inlineStr">
         <is>
-          <t>ROSSE Madeline</t>
+          <t>GUMUS Fatih</t>
         </is>
       </c>
       <c r="M46" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -1341,73 +1356,73 @@
           <t>M 1848/1</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>NETALA Frédéric</t>
-        </is>
-      </c>
-      <c r="E48" s="4" t="inlineStr">
+      <c r="C48" s="2" t="inlineStr">
         <is>
           <t>FRICKERT Florian</t>
         </is>
       </c>
+      <c r="E48" s="5" t="inlineStr">
+        <is>
+          <t>FRILLOT Jacky</t>
+        </is>
+      </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
-          <t>ECOMAC</t>
+          <t>CENTRE-POSE</t>
         </is>
       </c>
       <c r="H48" s="2" t="inlineStr">
         <is>
-          <t>VIAUD Cyril</t>
+          <t>TRAPANESE Antoine</t>
         </is>
       </c>
       <c r="I48" s="3" t="inlineStr">
         <is>
-          <t>RIGOT Sébastien</t>
-        </is>
-      </c>
-      <c r="J48" s="6" t="inlineStr">
+          <t>WEHRLEN Patrice</t>
+        </is>
+      </c>
+      <c r="J48" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="L48" s="2" t="inlineStr">
-        <is>
-          <t>BLATZ Jean-Marie</t>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>PASQUIER Alexandre</t>
         </is>
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>FRILLOT Jacky</t>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>SPITZ Eric</t>
         </is>
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>SPITZ Eric</t>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="D50" s="3" t="inlineStr">
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>RENCKER Michel</t>
+        </is>
+      </c>
+      <c r="E50" s="5" t="inlineStr">
         <is>
           <t>HUGG Christian</t>
         </is>
       </c>
-      <c r="E50" s="4" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
-        </is>
-      </c>
       <c r="L50" s="2" t="inlineStr">
         <is>
-          <t>CORSET Christo</t>
+          <t>FIGUEIREDO José</t>
         </is>
       </c>
       <c r="M50" s="1" t="inlineStr">
@@ -1425,86 +1440,91 @@
       </c>
       <c r="C52" s="2" t="inlineStr">
         <is>
+          <t>VILLEMIN Franck</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
           <t>GRIMONT Olivier</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
+      <c r="E52" s="5" t="inlineStr">
         <is>
           <t>FUCHS Eric</t>
         </is>
       </c>
-      <c r="E52" s="4" t="inlineStr">
-        <is>
-          <t>GAVROY Gilles</t>
-        </is>
-      </c>
       <c r="G52" s="1" t="inlineStr">
         <is>
-          <t>HST</t>
-        </is>
-      </c>
-      <c r="H52" s="6" t="inlineStr">
+          <t>ECOMAC</t>
+        </is>
+      </c>
+      <c r="H52" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="I52" s="6" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L52" s="2" t="inlineStr">
-        <is>
-          <t>BIELLMANN Cindy</t>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>VIAUD Cyril</t>
+        </is>
+      </c>
+      <c r="J52" s="5" t="inlineStr">
+        <is>
+          <t>RIGOT Sébastien</t>
+        </is>
+      </c>
+      <c r="L52" s="7" t="inlineStr">
+        <is>
+          <t>MARTIN Hugues</t>
         </is>
       </c>
       <c r="M52" s="1" t="inlineStr">
         <is>
-          <t>CP</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="C53" s="2" t="inlineStr">
         <is>
+          <t>DANIEL Jean-Luc</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
           <t>DA SILVA Axel</t>
         </is>
       </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>AUDREN Olivier</t>
-        </is>
-      </c>
-      <c r="E53" s="4" t="inlineStr">
-        <is>
-          <t>DANIEL Jean-Luc</t>
+      <c r="E53" s="5" t="inlineStr">
+        <is>
+          <t>FONTAINE Fabien</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="C54" s="2" t="inlineStr">
         <is>
+          <t>GAVROY Gilles</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
           <t>SCANDELLA Christophe</t>
         </is>
       </c>
-      <c r="D54" s="2" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
-        </is>
-      </c>
-      <c r="E54" s="4" t="inlineStr">
-        <is>
-          <t>MOZET Gaétan</t>
-        </is>
-      </c>
-      <c r="L54" s="2" t="inlineStr">
-        <is>
-          <t>GIDEMANN Olivier</t>
+      <c r="E54" s="5" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
+        </is>
+      </c>
+      <c r="L54" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PISKA Laurent </t>
         </is>
       </c>
       <c r="M54" s="1" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1517,41 +1537,46 @@
       </c>
       <c r="C56" s="2" t="inlineStr">
         <is>
-          <t>SCHWARZ Jean-Philippe</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>SAHLI Halim</t>
-        </is>
-      </c>
-      <c r="L56" s="2" t="inlineStr">
-        <is>
-          <t>GUMUS Fatih</t>
+          <t>KIEFFER Victor</t>
+        </is>
+      </c>
+      <c r="G56" s="1" t="inlineStr">
+        <is>
+          <t>HST</t>
+        </is>
+      </c>
+      <c r="H56" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="I56" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L56" s="5" t="inlineStr">
+        <is>
+          <t>FRITSCH Patrick</t>
         </is>
       </c>
       <c r="M56" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="C57" s="2" t="inlineStr">
         <is>
-          <t>FRITSCH Julien</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>LEDER Frédéric</t>
+          <t>MOZET Gaétan</t>
         </is>
       </c>
     </row>
     <row r="58">
-      <c r="L58" s="4" t="inlineStr">
-        <is>
-          <t>FIGUEIREDO José</t>
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>SIMLER Maurice</t>
         </is>
       </c>
       <c r="M58" s="1" t="inlineStr">
@@ -1561,66 +1586,22 @@
       </c>
     </row>
     <row r="59"/>
-    <row r="60">
-      <c r="B60" s="1" t="inlineStr">
-        <is>
-          <t>SRE</t>
-        </is>
-      </c>
-      <c r="L60" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PISKA Laurent </t>
-        </is>
-      </c>
-      <c r="M60" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-    </row>
+    <row r="60"/>
     <row r="61"/>
-    <row r="62">
-      <c r="L62" s="2" t="inlineStr">
-        <is>
-          <t>REIBEL Christophe</t>
-        </is>
-      </c>
-      <c r="M62" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-    </row>
+    <row r="62"/>
     <row r="63"/>
     <row r="64">
-      <c r="L64" s="2" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Pascal</t>
-        </is>
-      </c>
-      <c r="M64" s="1" t="inlineStr">
-        <is>
-          <t>*</t>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Personnel non affecté</t>
         </is>
       </c>
     </row>
     <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70">
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Personnel non affecté</t>
-        </is>
-      </c>
-    </row>
-    <row r="71"/>
-    <row r="72">
-      <c r="L72" s="4" t="inlineStr">
-        <is>
-          <t>RUBIO Alexandre</t>
+    <row r="66">
+      <c r="L66" s="8" t="inlineStr">
+        <is>
+          <t>Vincent WENDLING</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bug avec les préparateurs
</commit_message>
<xml_diff>
--- a/planning/static/excel/planning.xlsx
+++ b/planning/static/excel/planning.xlsx
@@ -35,18 +35,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF99FF99"/>
         <bgColor rgb="FF99FF99"/>
       </patternFill>
@@ -61,6 +49,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -106,12 +106,12 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="7" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="5" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="8" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="6" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,11 +488,11 @@
     <col customWidth="1" max="1" min="1" width="14.4"/>
     <col customWidth="1" max="2" min="2" width="22.8"/>
     <col customWidth="1" max="3" min="3" width="28.8"/>
-    <col customWidth="1" max="4" min="4" width="25.2"/>
-    <col customWidth="1" max="5" min="5" width="28.8"/>
+    <col customWidth="1" max="4" min="4" width="28.8"/>
+    <col customWidth="1" max="5" min="5" width="25.2"/>
     <col customWidth="1" max="6" min="6" width="7.199999999999999"/>
     <col customWidth="1" max="7" min="7" width="25.2"/>
-    <col customWidth="1" max="8" min="8" width="26.4"/>
+    <col customWidth="1" max="8" min="8" width="22.8"/>
     <col customWidth="1" max="9" min="9" width="27.6"/>
     <col customWidth="1" max="10" min="10" width="22.8"/>
     <col customWidth="1" max="11" min="11" width="7.199999999999999"/>
@@ -503,14 +503,14 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Semaine 19</t>
+          <t>Semaine 18</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MERCREDI</t>
+          <t>LUNDI</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
@@ -563,25 +563,30 @@
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
+          <t>DEPARIS Frédéric</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>REIBEL Christophe</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>FRITSCH Patrick</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>DEPARIS Frédéric</t>
-        </is>
-      </c>
       <c r="G4" s="1" t="inlineStr">
         <is>
           <t>SRE</t>
         </is>
       </c>
-      <c r="L4" s="4" t="inlineStr">
+      <c r="I4" s="3" t="inlineStr">
+        <is>
+          <t>SCHWARZ Jean-Philippe</t>
+        </is>
+      </c>
+      <c r="L4" s="2" t="inlineStr">
         <is>
           <t>DA COSTA Nelson</t>
         </is>
@@ -593,26 +598,26 @@
       </c>
     </row>
     <row r="5">
-      <c r="C5" s="5" t="inlineStr">
-        <is>
-          <t>SIMLER Maurice</t>
-        </is>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>PISKA Laurent</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
         <is>
           <t>WENDLING Christophe</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>PISKA Laurent</t>
-        </is>
-      </c>
     </row>
     <row r="6">
-      <c r="L6" s="4" t="inlineStr">
-        <is>
-          <t>FULLERINGER Gaétan</t>
+      <c r="L6" s="2" t="inlineStr">
+        <is>
+          <t>LOUIS Nicolas</t>
         </is>
       </c>
       <c r="M6" s="1" t="inlineStr">
@@ -628,21 +633,21 @@
           <t>B 1604</t>
         </is>
       </c>
-      <c r="C8" s="5" t="inlineStr">
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>BROGLIE Julien</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
         <is>
           <t>HELFTER Franck</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="E8" s="5" t="inlineStr">
         <is>
           <t>VINGATARAMIN Pierre</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>BROGLIE Julien</t>
-        </is>
-      </c>
       <c r="G8" s="1" t="inlineStr">
         <is>
           <t>SMT</t>
@@ -650,66 +655,66 @@
       </c>
       <c r="H8" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">ROTH Mathieu </t>
-        </is>
-      </c>
-      <c r="I8" s="6" t="inlineStr">
-        <is>
           <t xml:space="preserve">DJEBARA Philippe </t>
         </is>
       </c>
-      <c r="L8" s="4" t="inlineStr">
-        <is>
-          <t>LOUIS Nicolas</t>
+      <c r="I8" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L8" s="2" t="inlineStr">
+        <is>
+          <t>YEGEN Zulkifar</t>
         </is>
       </c>
       <c r="M8" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="C9" s="5" t="inlineStr">
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WOELFFLIN Gregory </t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
         <is>
           <t>SCHILLINGER  Jérémy</t>
         </is>
       </c>
-      <c r="D9" s="3" t="inlineStr">
+      <c r="E9" s="5" t="inlineStr">
         <is>
           <t>HORACEK Julien</t>
         </is>
       </c>
-      <c r="E9" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
     </row>
     <row r="10">
-      <c r="C10" s="5" t="inlineStr">
+      <c r="C10" s="7" t="inlineStr">
+        <is>
+          <t>Intérimaire</t>
+        </is>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
         <is>
           <t>CAMARASA Sébastien</t>
         </is>
       </c>
-      <c r="D10" s="3" t="inlineStr">
+      <c r="E10" s="5" t="inlineStr">
         <is>
           <t>HUEBER Olivier</t>
         </is>
       </c>
-      <c r="E10" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L10" s="4" t="inlineStr">
-        <is>
-          <t>MOSCOPOULOS Sébastien</t>
+      <c r="L10" s="8" t="inlineStr">
+        <is>
+          <t>DA SILVA David</t>
         </is>
       </c>
       <c r="M10" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -720,29 +725,29 @@
           <t>B 2100</t>
         </is>
       </c>
-      <c r="C12" s="5" t="inlineStr">
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>MORENO José</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>DUCROT Déborah</t>
         </is>
       </c>
-      <c r="D12" s="3" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>LUDAESCHER Olivier</t>
         </is>
       </c>
-      <c r="E12" s="4" t="inlineStr">
-        <is>
-          <t>MORENO José</t>
-        </is>
-      </c>
       <c r="G12" s="1" t="inlineStr">
         <is>
           <t>LBB1</t>
         </is>
       </c>
-      <c r="L12" s="4" t="inlineStr">
-        <is>
-          <t>SPIELMANN Patrice</t>
+      <c r="L12" s="5" t="inlineStr">
+        <is>
+          <t>BAUMANN Dylan</t>
         </is>
       </c>
       <c r="M12" s="1" t="inlineStr">
@@ -752,46 +757,46 @@
       </c>
     </row>
     <row r="13">
-      <c r="C13" s="5" t="inlineStr">
-        <is>
-          <t>ROUSSIN Frédéric</t>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>ABELLAN GRINAN Laurent</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
+          <t>LUDAESCHER Pascal</t>
+        </is>
+      </c>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
           <t>HAAG Patrick</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr">
-        <is>
-          <t>ABELLAN GRINAN Laurent</t>
-        </is>
-      </c>
     </row>
     <row r="14">
-      <c r="C14" s="5" t="inlineStr">
-        <is>
-          <t>LICHTLE Jean-Sébastien</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>SCHAAL Eric</t>
+        </is>
+      </c>
+      <c r="D14" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KOESSEL Marc </t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
         <is>
           <t>CASPAR Gaël</t>
         </is>
       </c>
-      <c r="E14" s="4" t="inlineStr">
-        <is>
-          <t>SCHAAL Eric</t>
-        </is>
-      </c>
-      <c r="L14" s="4" t="inlineStr">
-        <is>
-          <t>TRAPANESE Antoine</t>
+      <c r="L14" s="5" t="inlineStr">
+        <is>
+          <t>ACKERMANN Rémy</t>
         </is>
       </c>
       <c r="M14" s="1" t="inlineStr">
         <is>
-          <t>rcn</t>
+          <t>am</t>
         </is>
       </c>
     </row>
@@ -802,7 +807,12 @@
           <t>B2000</t>
         </is>
       </c>
-      <c r="D16" s="3" t="inlineStr">
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>RUBIO Alexandre</t>
+        </is>
+      </c>
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>SIGWALT Thierry</t>
         </is>
@@ -812,38 +822,43 @@
           <t>MITRAILLEUSE</t>
         </is>
       </c>
-      <c r="I16" s="6" t="inlineStr">
+      <c r="H16" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">PINTO José </t>
         </is>
       </c>
-      <c r="L16" s="4" t="inlineStr">
+      <c r="L16" s="5" t="inlineStr">
+        <is>
+          <t>AUDREN Olivier</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" s="2" t="inlineStr">
         <is>
           <t>WITZ Alain</t>
         </is>
       </c>
-      <c r="M16" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="5" t="inlineStr">
-        <is>
-          <t>NESZCZADYN Franck</t>
+      <c r="E17" s="5" t="inlineStr">
+        <is>
+          <t>SIMON Gael</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="L18" s="4" t="inlineStr">
-        <is>
-          <t>YEGEN Zulkifar</t>
+      <c r="L18" s="5" t="inlineStr">
+        <is>
+          <t>BELIANE Karim</t>
         </is>
       </c>
       <c r="M18" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -854,24 +869,29 @@
           <t>G 1628</t>
         </is>
       </c>
-      <c r="D20" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">WOELFFLIN Gregory </t>
-        </is>
-      </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="C20" s="2" t="inlineStr">
         <is>
           <t>FOECHTERLE Jean</t>
         </is>
       </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>NESZCZADYN Franck</t>
+        </is>
+      </c>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>BUCHER Cyril</t>
+        </is>
+      </c>
       <c r="G20" s="1" t="inlineStr">
         <is>
           <t>MITR. BIMAC</t>
         </is>
       </c>
-      <c r="L20" s="7" t="inlineStr">
-        <is>
-          <t>DA SILVA David</t>
+      <c r="L20" s="5" t="inlineStr">
+        <is>
+          <t>EBRAN Vincent</t>
         </is>
       </c>
       <c r="M20" s="1" t="inlineStr">
@@ -881,36 +901,46 @@
       </c>
     </row>
     <row r="21">
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>FULLERINGER Gaétan</t>
+        </is>
+      </c>
       <c r="D21" s="3" t="inlineStr">
         <is>
+          <t>BLATZ Jean-Marie</t>
+        </is>
+      </c>
+      <c r="E21" s="5" t="inlineStr">
+        <is>
           <t>GEIGER Frédéric</t>
         </is>
       </c>
-      <c r="E21" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
     </row>
     <row r="22">
-      <c r="D22" s="8" t="inlineStr">
+      <c r="C22" s="7" t="inlineStr">
         <is>
           <t>Intérimaire</t>
         </is>
       </c>
-      <c r="E22" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L22" s="4" t="inlineStr">
-        <is>
-          <t>FERDER Thomas</t>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>LICHTLE Jean-Sébastien</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t>SAHLI Halim</t>
+        </is>
+      </c>
+      <c r="L22" s="5" t="inlineStr">
+        <is>
+          <t>HAIL Fehrat</t>
         </is>
       </c>
       <c r="M22" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -921,19 +951,19 @@
           <t>DOMINO</t>
         </is>
       </c>
-      <c r="C24" s="5" t="inlineStr">
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>SPIELMANN Patrice</t>
+        </is>
+      </c>
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>BERGER Virgil</t>
         </is>
       </c>
-      <c r="D24" s="3" t="inlineStr">
-        <is>
-          <t>BAUMANN Dylan</t>
-        </is>
-      </c>
-      <c r="E24" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">KOESSEL Marc </t>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
       <c r="G24" s="1" t="inlineStr">
@@ -941,42 +971,42 @@
           <t>MANUTENTION INTÉGRÉ</t>
         </is>
       </c>
-      <c r="H24" s="5" t="inlineStr">
+      <c r="H24" s="2" t="inlineStr">
+        <is>
+          <t>HOFFERT Patrick</t>
+        </is>
+      </c>
+      <c r="I24" s="3" t="inlineStr">
         <is>
           <t>BAUMANN Mike</t>
         </is>
       </c>
-      <c r="I24" s="3" t="inlineStr">
+      <c r="J24" s="5" t="inlineStr">
         <is>
           <t>RAMON Dominique</t>
         </is>
       </c>
-      <c r="J24" s="4" t="inlineStr">
-        <is>
-          <t>HOFFERT Patrick</t>
-        </is>
-      </c>
-      <c r="L24" s="7" t="inlineStr">
-        <is>
-          <t>GURLER ONUR</t>
+      <c r="L24" s="5" t="inlineStr">
+        <is>
+          <t>HIRSINGER Pascal</t>
         </is>
       </c>
       <c r="M24" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>rc</t>
         </is>
       </c>
     </row>
     <row r="25"/>
     <row r="26">
-      <c r="L26" s="4" t="inlineStr">
-        <is>
-          <t>LIER Romain</t>
+      <c r="L26" s="5" t="inlineStr">
+        <is>
+          <t>NETALA Frédéric</t>
         </is>
       </c>
       <c r="M26" s="1" t="inlineStr">
         <is>
-          <t>R</t>
+          <t>rtt</t>
         </is>
       </c>
     </row>
@@ -987,49 +1017,49 @@
           <t>PRESSE À BALLE</t>
         </is>
       </c>
-      <c r="C28" s="4" t="inlineStr">
-        <is>
-          <t>RITT Jean Jacques</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="inlineStr">
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>MULLER Gilbert</t>
+        </is>
+      </c>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>RAKOTONDRAMANANA Nivo</t>
+        </is>
+      </c>
+      <c r="E28" s="5" t="inlineStr">
+        <is>
+          <t>SCHREIBER Bertrand</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>PRÉPARATEUR</t>
+        </is>
+      </c>
+      <c r="H28" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="E28" s="4" t="inlineStr">
-        <is>
-          <t>MULLER Gilbert</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="inlineStr">
-        <is>
-          <t>PRÉPARATEUR</t>
-        </is>
-      </c>
-      <c r="H28" s="2" t="inlineStr">
+      <c r="I28" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="I28" s="2" t="inlineStr">
+      <c r="J28" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="J28" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L28" s="4" t="inlineStr">
-        <is>
-          <t>VILLEMIN Franck</t>
+      <c r="L28" s="5" t="inlineStr">
+        <is>
+          <t>ROGLER Richard</t>
         </is>
       </c>
       <c r="M28" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>D</t>
         </is>
       </c>
     </row>
@@ -1037,12 +1067,12 @@
     <row r="30">
       <c r="L30" s="3" t="inlineStr">
         <is>
-          <t>BUCHER Cyril</t>
+          <t>CORSET Christo</t>
         </is>
       </c>
       <c r="M30" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -1058,43 +1088,43 @@
           <t>M 1228</t>
         </is>
       </c>
-      <c r="H32" s="5" t="inlineStr">
+      <c r="H32" s="2" t="inlineStr">
+        <is>
+          <t>FRICKERT Rémy</t>
+        </is>
+      </c>
+      <c r="I32" s="3" t="inlineStr">
         <is>
           <t>GRASSIN Axel</t>
         </is>
       </c>
-      <c r="J32" s="4" t="inlineStr">
-        <is>
-          <t>FRICKERT Rémy</t>
-        </is>
-      </c>
       <c r="L32" s="3" t="inlineStr">
         <is>
-          <t>SIMON Gael</t>
+          <t>LEROY Nicolas</t>
         </is>
       </c>
       <c r="M32" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="H33" s="2" t="inlineStr">
         <is>
+          <t>GURLER Onur</t>
+        </is>
+      </c>
+      <c r="I33" s="4" t="inlineStr">
+        <is>
           <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="J33" s="4" t="inlineStr">
-        <is>
-          <t>GURLER Onur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="L34" s="3" t="inlineStr">
         <is>
-          <t>SCHREIBER Bertrand</t>
+          <t>ROUSSIN Frédéric</t>
         </is>
       </c>
       <c r="M34" s="1" t="inlineStr">
@@ -1110,64 +1140,64 @@
           <t>EMBALLAGE</t>
         </is>
       </c>
-      <c r="C36" s="5" t="inlineStr">
-        <is>
-          <t>LEROY Nicolas</t>
-        </is>
-      </c>
-      <c r="D36" s="3" t="inlineStr">
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>GANTNER Stéphane</t>
+        </is>
+      </c>
+      <c r="D36" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ROTH Mathieu </t>
+        </is>
+      </c>
+      <c r="E36" s="5" t="inlineStr">
         <is>
           <t>SUTTER Thierry</t>
         </is>
       </c>
-      <c r="E36" s="4" t="inlineStr">
-        <is>
-          <t>GANTNER Stéphane</t>
-        </is>
-      </c>
       <c r="G36" s="1" t="inlineStr">
         <is>
           <t>M 924</t>
         </is>
       </c>
-      <c r="H36" s="5" t="inlineStr">
-        <is>
-          <t>ANDRZEJEWSKI Nicolas</t>
-        </is>
-      </c>
-      <c r="I36" s="3" t="inlineStr">
-        <is>
-          <t>HIRSINGER Pascal</t>
-        </is>
-      </c>
-      <c r="J36" s="4" t="inlineStr">
+      <c r="H36" s="2" t="inlineStr">
         <is>
           <t>RUDLOFF Jérémy</t>
         </is>
       </c>
-      <c r="L36" s="3" t="inlineStr">
-        <is>
-          <t>BELIANE Karim</t>
+      <c r="I36" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="J36" s="5" t="inlineStr">
+        <is>
+          <t>HILDWEIN Steve</t>
+        </is>
+      </c>
+      <c r="L36" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SHULER Evelyne </t>
         </is>
       </c>
       <c r="M36" s="1" t="inlineStr">
         <is>
-          <t>rtt</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="H37" s="5" t="inlineStr">
+      <c r="H37" s="3" t="inlineStr">
         <is>
           <t>HERMANN Cédric</t>
         </is>
       </c>
-      <c r="I37" s="3" t="inlineStr">
-        <is>
-          <t>HILDWEIN Steve</t>
-        </is>
-      </c>
-      <c r="J37" s="2" t="inlineStr">
+      <c r="I37" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="J37" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
@@ -1176,7 +1206,7 @@
     <row r="38">
       <c r="L38" s="3" t="inlineStr">
         <is>
-          <t>CAMACHO Michel</t>
+          <t>ANDRZEJEWSKI Nicolas</t>
         </is>
       </c>
       <c r="M38" s="1" t="inlineStr">
@@ -1192,78 +1222,68 @@
           <t>MANUTENTION LOURD</t>
         </is>
       </c>
-      <c r="C40" s="6" t="inlineStr">
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>MOSCOPOULOS Sébastien</t>
+        </is>
+      </c>
+      <c r="D40" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">BOIREAU Stéphane </t>
         </is>
       </c>
-      <c r="D40" s="3" t="inlineStr">
+      <c r="E40" s="5" t="inlineStr">
         <is>
           <t>MOEGLING Vincent</t>
         </is>
       </c>
-      <c r="E40" s="4" t="inlineStr">
-        <is>
-          <t>SCHENCK Emmanuel</t>
-        </is>
-      </c>
       <c r="G40" s="1" t="inlineStr">
         <is>
           <t>M 718</t>
         </is>
       </c>
-      <c r="H40" s="5" t="inlineStr">
+      <c r="H40" s="2" t="inlineStr">
+        <is>
+          <t>FERDER Thomas</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
         <is>
           <t>MASSINON Frédéric</t>
         </is>
       </c>
-      <c r="I40" s="3" t="inlineStr">
-        <is>
-          <t>RAKOTONDRAMANANA Nivo</t>
-        </is>
-      </c>
-      <c r="J40" s="4" t="inlineStr">
-        <is>
-          <t>CORNOT David</t>
-        </is>
-      </c>
       <c r="L40" s="3" t="inlineStr">
         <is>
-          <t>EBRAN Vincent</t>
+          <t>BIELLMANN Cindy</t>
         </is>
       </c>
       <c r="M40" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>CP</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="H41" s="5" t="inlineStr">
-        <is>
-          <t>PASQUIER Alexandre</t>
-        </is>
-      </c>
-      <c r="I41" s="3" t="inlineStr">
-        <is>
-          <t>ACKERMANN Rémy</t>
-        </is>
-      </c>
-      <c r="J41" s="4" t="inlineStr">
+      <c r="H41" s="2" t="inlineStr">
         <is>
           <t>ZWICKERT Xavier</t>
+        </is>
+      </c>
+      <c r="I41" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="L42" s="3" t="inlineStr">
         <is>
-          <t>FONTAINE Fabien</t>
+          <t>FRITSCH Julien</t>
         </is>
       </c>
       <c r="M42" s="1" t="inlineStr">
         <is>
-          <t>rc</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1274,9 +1294,9 @@
           <t>2T</t>
         </is>
       </c>
-      <c r="C44" s="8" t="inlineStr">
-        <is>
-          <t>Vincent WENDLING</t>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>SCHENCK Emmanuel</t>
         </is>
       </c>
       <c r="G44" s="1" t="inlineStr">
@@ -1286,36 +1306,46 @@
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>Poste non affecté</t>
+          <t>CORNOT David</t>
+        </is>
+      </c>
+      <c r="J44" s="5" t="inlineStr">
+        <is>
+          <t>CAMACHO Michel</t>
         </is>
       </c>
       <c r="L44" s="3" t="inlineStr">
         <is>
-          <t>HAIL Fehrat</t>
+          <t>GIDEMANN Olivier</t>
         </is>
       </c>
       <c r="M44" s="1" t="inlineStr">
         <is>
-          <t>M</t>
+          <t>C</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>Poste non affecté</t>
+          <t>LIER Romain</t>
+        </is>
+      </c>
+      <c r="J45" s="5" t="inlineStr">
+        <is>
+          <t>ROSSE Madeline</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="L46" s="3" t="inlineStr">
         <is>
-          <t>ROSSE Madeline</t>
+          <t>GUMUS Fatih</t>
         </is>
       </c>
       <c r="M46" s="1" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>M</t>
         </is>
       </c>
     </row>
@@ -1326,73 +1356,73 @@
           <t>M 1848/1</t>
         </is>
       </c>
-      <c r="D48" s="3" t="inlineStr">
-        <is>
-          <t>NETALA Frédéric</t>
-        </is>
-      </c>
-      <c r="E48" s="4" t="inlineStr">
+      <c r="C48" s="2" t="inlineStr">
         <is>
           <t>FRICKERT Florian</t>
         </is>
       </c>
+      <c r="E48" s="5" t="inlineStr">
+        <is>
+          <t>FRILLOT Jacky</t>
+        </is>
+      </c>
       <c r="G48" s="1" t="inlineStr">
         <is>
           <t>CENTRE-POSE</t>
         </is>
       </c>
-      <c r="H48" s="5" t="inlineStr">
+      <c r="H48" s="2" t="inlineStr">
+        <is>
+          <t>TRAPANESE Antoine</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
         <is>
           <t>WEHRLEN Patrice</t>
         </is>
       </c>
-      <c r="I48" s="3" t="inlineStr">
-        <is>
-          <t>ROGLER Richard</t>
-        </is>
-      </c>
       <c r="J48" s="4" t="inlineStr">
         <is>
-          <t>KIEFFER Victor</t>
-        </is>
-      </c>
-      <c r="L48" s="5" t="inlineStr">
-        <is>
-          <t>BLATZ Jean-Marie</t>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="L48" s="3" t="inlineStr">
+        <is>
+          <t>PASQUIER Alexandre</t>
         </is>
       </c>
       <c r="M48" s="1" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>R</t>
         </is>
       </c>
     </row>
     <row r="49">
-      <c r="D49" s="3" t="inlineStr">
-        <is>
-          <t>FRILLOT Jacky</t>
+      <c r="C49" s="2" t="inlineStr">
+        <is>
+          <t>SPITZ Eric</t>
         </is>
       </c>
       <c r="E49" s="4" t="inlineStr">
         <is>
-          <t>SPITZ Eric</t>
+          <t>Poste non affecté</t>
         </is>
       </c>
     </row>
     <row r="50">
-      <c r="D50" s="3" t="inlineStr">
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>RENCKER Michel</t>
+        </is>
+      </c>
+      <c r="E50" s="5" t="inlineStr">
         <is>
           <t>HUGG Christian</t>
         </is>
       </c>
-      <c r="E50" s="4" t="inlineStr">
-        <is>
-          <t>RENCKER Michel</t>
-        </is>
-      </c>
-      <c r="L50" s="5" t="inlineStr">
-        <is>
-          <t>CORSET Christo</t>
+      <c r="L50" s="2" t="inlineStr">
+        <is>
+          <t>FIGUEIREDO José</t>
         </is>
       </c>
       <c r="M50" s="1" t="inlineStr">
@@ -1408,93 +1438,93 @@
           <t>M 1848/2</t>
         </is>
       </c>
-      <c r="C52" s="5" t="inlineStr">
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>VILLEMIN Franck</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
         <is>
           <t>GRIMONT Olivier</t>
         </is>
       </c>
-      <c r="D52" s="3" t="inlineStr">
+      <c r="E52" s="5" t="inlineStr">
         <is>
           <t>FUCHS Eric</t>
         </is>
       </c>
-      <c r="E52" s="4" t="inlineStr">
+      <c r="G52" s="1" t="inlineStr">
+        <is>
+          <t>ECOMAC</t>
+        </is>
+      </c>
+      <c r="H52" s="4" t="inlineStr">
+        <is>
+          <t>Poste non affecté</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>VIAUD Cyril</t>
+        </is>
+      </c>
+      <c r="J52" s="5" t="inlineStr">
+        <is>
+          <t>RIGOT Sébastien</t>
+        </is>
+      </c>
+      <c r="L52" s="8" t="inlineStr">
+        <is>
+          <t>MARTIN Hugues</t>
+        </is>
+      </c>
+      <c r="M52" s="1" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="C53" s="2" t="inlineStr">
+        <is>
+          <t>DANIEL Jean-Luc</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>DA SILVA Axel</t>
+        </is>
+      </c>
+      <c r="E53" s="5" t="inlineStr">
+        <is>
+          <t>FONTAINE Fabien</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="C54" s="2" t="inlineStr">
         <is>
           <t>GAVROY Gilles</t>
         </is>
       </c>
-      <c r="G52" s="1" t="inlineStr">
-        <is>
-          <t>ECOMAC</t>
-        </is>
-      </c>
-      <c r="H52" s="5" t="inlineStr">
-        <is>
-          <t>VIAUD Cyril</t>
-        </is>
-      </c>
-      <c r="I52" s="3" t="inlineStr">
-        <is>
-          <t>RIGOT Sébastien</t>
-        </is>
-      </c>
-      <c r="J52" s="2" t="inlineStr">
-        <is>
-          <t>Poste non affecté</t>
-        </is>
-      </c>
-      <c r="L52" s="5" t="inlineStr">
-        <is>
-          <t>BIELLMANN Cindy</t>
-        </is>
-      </c>
-      <c r="M52" s="1" t="inlineStr">
-        <is>
-          <t>CP</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="C53" s="5" t="inlineStr">
-        <is>
-          <t>DA SILVA Axel</t>
-        </is>
-      </c>
-      <c r="D53" s="3" t="inlineStr">
-        <is>
-          <t>AUDREN Olivier</t>
-        </is>
-      </c>
-      <c r="E53" s="4" t="inlineStr">
-        <is>
-          <t>DANIEL Jean-Luc</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="C54" s="5" t="inlineStr">
+      <c r="D54" s="3" t="inlineStr">
         <is>
           <t>SCANDELLA Christophe</t>
         </is>
       </c>
-      <c r="D54" s="8" t="inlineStr">
-        <is>
-          <t>Intérimaire</t>
-        </is>
-      </c>
-      <c r="E54" s="4" t="inlineStr">
-        <is>
-          <t>MOZET Gaétan</t>
-        </is>
-      </c>
-      <c r="L54" s="5" t="inlineStr">
-        <is>
-          <t>GIDEMANN Olivier</t>
+      <c r="E54" s="5" t="inlineStr">
+        <is>
+          <t>LEDER Frédéric</t>
+        </is>
+      </c>
+      <c r="L54" s="8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PISKA Laurent </t>
         </is>
       </c>
       <c r="M54" s="1" t="inlineStr">
         <is>
-          <t>GE</t>
+          <t>C</t>
         </is>
       </c>
     </row>
@@ -1505,14 +1535,9 @@
           <t>TCY</t>
         </is>
       </c>
-      <c r="C56" s="5" t="inlineStr">
-        <is>
-          <t>SCHWARZ Jean-Philippe</t>
-        </is>
-      </c>
-      <c r="D56" s="3" t="inlineStr">
-        <is>
-          <t>SAHLI Halim</t>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>KIEFFER Victor</t>
         </is>
       </c>
       <c r="G56" s="1" t="inlineStr">
@@ -1520,107 +1545,63 @@
           <t>HST</t>
         </is>
       </c>
-      <c r="H56" s="2" t="inlineStr">
+      <c r="H56" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
-      <c r="I56" s="2" t="inlineStr">
+      <c r="I56" s="4" t="inlineStr">
         <is>
           <t>Poste non affecté</t>
         </is>
       </c>
       <c r="L56" s="5" t="inlineStr">
         <is>
-          <t>GUMUS Fatih</t>
+          <t>FRITSCH Patrick</t>
         </is>
       </c>
       <c r="M56" s="1" t="inlineStr">
         <is>
+          <t>R</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="C57" s="2" t="inlineStr">
+        <is>
+          <t>MOZET Gaétan</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="L58" s="3" t="inlineStr">
+        <is>
+          <t>SIMLER Maurice</t>
+        </is>
+      </c>
+      <c r="M58" s="1" t="inlineStr">
+        <is>
           <t>M</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="C57" s="5" t="inlineStr">
-        <is>
-          <t>FRITSCH Julien</t>
-        </is>
-      </c>
-      <c r="D57" s="3" t="inlineStr">
-        <is>
-          <t>LEDER Frédéric</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="L58" s="4" t="inlineStr">
-        <is>
-          <t>FIGUEIREDO José</t>
-        </is>
-      </c>
-      <c r="M58" s="1" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-    </row>
     <row r="59"/>
-    <row r="60">
-      <c r="L60" s="7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">PISKA Laurent </t>
-        </is>
-      </c>
-      <c r="M60" s="1" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-    </row>
+    <row r="60"/>
     <row r="61"/>
-    <row r="62">
-      <c r="L62" s="5" t="inlineStr">
-        <is>
-          <t>REIBEL Christophe</t>
-        </is>
-      </c>
-      <c r="M62" s="1" t="inlineStr">
-        <is>
-          <t>R</t>
-        </is>
-      </c>
-    </row>
+    <row r="62"/>
     <row r="63"/>
     <row r="64">
-      <c r="L64" s="5" t="inlineStr">
-        <is>
-          <t>LUDAESCHER Pascal</t>
-        </is>
-      </c>
-      <c r="M64" s="1" t="inlineStr">
-        <is>
-          <t>*</t>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Personnel non affecté</t>
         </is>
       </c>
     </row>
     <row r="65"/>
-    <row r="66"/>
-    <row r="67"/>
-    <row r="68"/>
-    <row r="69"/>
-    <row r="70">
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Personnel non affecté</t>
-        </is>
-      </c>
-    </row>
-    <row r="71"/>
-    <row r="72">
-      <c r="L72" s="4" t="inlineStr">
-        <is>
-          <t>RUBIO Alexandre</t>
+    <row r="66">
+      <c r="L66" s="7" t="inlineStr">
+        <is>
+          <t>Vincent WENDLING</t>
         </is>
       </c>
     </row>

</xml_diff>